<commit_message>
select/where expressions and rename
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Uni\DataEngineering\WS22\Guided Research\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260417FF-C3E7-4477-A148-2253B9632789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF73C27A-942E-4309-9389-08794CFB52D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="2400" windowWidth="21600" windowHeight="11775" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
+    <workbookView xWindow="3180" yWindow="2400" windowWidth="21600" windowHeight="11775" activeTab="1" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
   <sheets>
     <sheet name="Meeting Notes" sheetId="4" r:id="rId1"/>
-    <sheet name="Papers" sheetId="1" r:id="rId2"/>
-    <sheet name="Parsers" sheetId="2" r:id="rId3"/>
-    <sheet name="Optimizers" sheetId="3" r:id="rId4"/>
+    <sheet name="SQL Parser" sheetId="5" r:id="rId2"/>
+    <sheet name="Papers" sheetId="1" r:id="rId3"/>
+    <sheet name="Parsers" sheetId="2" r:id="rId4"/>
+    <sheet name="Optimizers" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="226">
   <si>
     <t>paper</t>
   </si>
@@ -623,12 +624,117 @@
 Add decorrelation optimization (basic optimizer, detect depedent joins, decorrelating algorithm)
 In Future add table schema as input</t>
   </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>column ref</t>
+  </si>
+  <si>
+    <t>alias</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>agg functions</t>
+  </si>
+  <si>
+    <t>rename</t>
+  </si>
+  <si>
+    <t>expressions</t>
+  </si>
+  <si>
+    <t>case</t>
+  </si>
+  <si>
+    <t>where</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>no relation</t>
+  </si>
+  <si>
+    <t>cross product</t>
+  </si>
+  <si>
+    <t>subqueries</t>
+  </si>
+  <si>
+    <t>joins</t>
+  </si>
+  <si>
+    <t>consts</t>
+  </si>
+  <si>
+    <t>AND/OR/NOT</t>
+  </si>
+  <si>
+    <t>exists</t>
+  </si>
+  <si>
+    <t>between</t>
+  </si>
+  <si>
+    <t>parenthesis</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>group by</t>
+  </si>
+  <si>
+    <t>having</t>
+  </si>
+  <si>
+    <t>order by</t>
+  </si>
+  <si>
+    <t>asc</t>
+  </si>
+  <si>
+    <t>desc</t>
+  </si>
+  <si>
+    <t>interval</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>like</t>
+  </si>
+  <si>
+    <t>views</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>substring</t>
+  </si>
+  <si>
+    <t>questions</t>
+  </si>
+  <si>
+    <t>case when… to RA?</t>
+  </si>
+  <si>
+    <t>is RA rename operator needed? Just integrate into projection</t>
+  </si>
+  <si>
+    <t>can integrate function evaluation into projection?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -650,8 +756,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -661,6 +775,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -678,7 +804,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -693,6 +819,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1010,19 +1142,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FDCCB2-898C-4E8A-AEF1-A7FCAFD38A4A}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.109375" style="4" customWidth="1"/>
-    <col min="2" max="2" width="55.5546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="65.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="4"/>
+    <col min="1" max="1" width="24.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="55.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="65.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>176</v>
       </c>
@@ -1033,7 +1165,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>175</v>
       </c>
@@ -1044,7 +1176,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>179</v>
       </c>
@@ -1052,7 +1184,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>183</v>
       </c>
@@ -1060,7 +1192,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>182</v>
       </c>
@@ -1068,7 +1200,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>185</v>
       </c>
@@ -1076,7 +1208,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>189</v>
       </c>
@@ -1084,7 +1216,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>187</v>
       </c>
@@ -1099,6 +1231,179 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C36143C-8755-4841-9383-2CD561E91E02}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" t="s">
+        <v>192</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="I2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="D3" t="s">
+        <v>212</v>
+      </c>
+      <c r="E3" t="s">
+        <v>214</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="I3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="E4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="I4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="F5" s="10"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B6" t="s">
+        <v>204</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="11" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C530AA-EE6D-4730-B7FC-66C1C2338D8E}">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -1106,17 +1411,17 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="38" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="62.88671875" customWidth="1"/>
+    <col min="6" max="6" width="62.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1136,7 +1441,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1153,7 +1458,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1170,7 +1475,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1187,7 +1492,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1204,7 +1509,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -1221,7 +1526,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1241,7 +1546,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1261,7 +1566,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -1281,7 +1586,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1298,7 +1603,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1315,7 +1620,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1335,7 +1640,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -1355,7 +1660,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -1372,7 +1677,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -1392,7 +1697,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -1409,7 +1714,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -1429,7 +1734,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -1449,7 +1754,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -1466,7 +1771,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -1501,7 +1806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800A685A-9F16-4D2A-89B8-E0E1402FCD61}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -1509,18 +1814,18 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="49.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>77</v>
       </c>
@@ -1543,7 +1848,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -1563,7 +1868,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1583,7 +1888,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -1606,7 +1911,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -1629,7 +1934,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -1649,7 +1954,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -1672,7 +1977,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -1695,7 +2000,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>113</v>
       </c>
@@ -1715,7 +2020,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -1735,7 +2040,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>130</v>
       </c>
@@ -1758,7 +2063,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>153</v>
       </c>
@@ -1781,7 +2086,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>157</v>
       </c>
@@ -1804,7 +2109,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>115</v>
       </c>
@@ -1812,7 +2117,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>121</v>
       </c>
@@ -1823,7 +2128,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -1834,7 +2139,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>135</v>
       </c>
@@ -1845,7 +2150,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>125</v>
       </c>
@@ -1869,7 +2174,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D31B28C7-0856-B849-8670-D0B5AB075FAE}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -1877,13 +2182,13 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="37.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.88671875" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>136</v>
       </c>
@@ -1900,7 +2205,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -1917,7 +2222,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>142</v>
       </c>
@@ -1931,7 +2236,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>146</v>
       </c>
@@ -1942,7 +2247,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>167</v>
       </c>

</xml_diff>

<commit_message>
where clause bool parenthesis
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Uni\DataEngineering\WS22\Guided Research\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8D0FA9-A5DC-4CF7-9444-22384E252987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B42BFE-5D27-48A3-AD69-D989B2F54C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20625" yWindow="1740" windowWidth="14325" windowHeight="11775" activeTab="1" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
+    <workbookView xWindow="19305" yWindow="1740" windowWidth="14325" windowHeight="11775" activeTab="1" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
   <sheets>
     <sheet name="Meeting Notes" sheetId="4" r:id="rId1"/>
@@ -1263,7 +1263,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,8 +1314,8 @@
       <c r="E2" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="F2" t="s">
-        <v>217</v>
+      <c r="F2" s="9" t="s">
+        <v>230</v>
       </c>
       <c r="I2" t="s">
         <v>222</v>
@@ -1338,7 +1338,7 @@
         <v>213</v>
       </c>
       <c r="F3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I3" t="s">
         <v>223</v>
@@ -1358,7 +1358,7 @@
         <v>214</v>
       </c>
       <c r="F4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="I4" t="s">
         <v>224</v>
@@ -1377,8 +1377,8 @@
       <c r="C5" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>230</v>
+      <c r="F5" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1396,8 +1396,8 @@
       <c r="A7" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>206</v>
+      <c r="C7" s="9" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -1405,7 +1405,7 @@
         <v>226</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1413,12 +1413,12 @@
         <v>197</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C10" s="10" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
parse correlated Q1 and Q2
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Uni\DataEngineering\WS22\Guided Research\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B42BFE-5D27-48A3-AD69-D989B2F54C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E67F1D2-B472-413A-9589-579B9E115F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19305" yWindow="1740" windowWidth="14325" windowHeight="11775" activeTab="1" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="240">
   <si>
     <t>paper</t>
   </si>
@@ -670,9 +670,6 @@
     <t>AND/OR/NOT</t>
   </si>
   <si>
-    <t>exists</t>
-  </si>
-  <si>
     <t>between</t>
   </si>
   <si>
@@ -691,12 +688,6 @@
     <t>order by</t>
   </si>
   <si>
-    <t>asc</t>
-  </si>
-  <si>
-    <t>desc</t>
-  </si>
-  <si>
     <t>interval</t>
   </si>
   <si>
@@ -709,9 +700,6 @@
     <t>views</t>
   </si>
   <si>
-    <t>in</t>
-  </si>
-  <si>
     <t>substring</t>
   </si>
   <si>
@@ -733,16 +721,55 @@
     <t>agg functions (no group by)</t>
   </si>
   <si>
-    <t>2, 4, 17, 20, 21, 22</t>
-  </si>
-  <si>
-    <t>TPCH Correlated Subqueries</t>
-  </si>
-  <si>
     <t>correlated subqueries</t>
   </si>
   <si>
     <t>print RA tree</t>
+  </si>
+  <si>
+    <t>can integrate group/order by into projection?</t>
+  </si>
+  <si>
+    <t>(-) column ref</t>
+  </si>
+  <si>
+    <t>limit</t>
+  </si>
+  <si>
+    <t>can we assume we are working with sets?</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>Figure 8: what is map operator and selection doing?</t>
+  </si>
+  <si>
+    <t>25.10.2022</t>
+  </si>
+  <si>
+    <t>Parsing correlated queries into dependent join</t>
+  </si>
+  <si>
+    <t>Doesn't make sense to introduce dependent join in step 3, because then already decorrelated</t>
+  </si>
+  <si>
+    <t>exists (use DJ)</t>
+  </si>
+  <si>
+    <t>in (use DJ)</t>
+  </si>
+  <si>
+    <t>Neumann Q1, Q2</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>TPCH Correlated</t>
   </si>
 </sst>
 </file>
@@ -831,7 +858,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -853,6 +880,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1168,10 +1196,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FDCCB2-898C-4E8A-AEF1-A7FCAFD38A4A}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1252,6 +1280,17 @@
         <v>188</v>
       </c>
     </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1260,10 +1299,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C36143C-8755-4841-9383-2CD561E91E02}">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,16 +1325,16 @@
         <v>198</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1308,17 +1347,17 @@
       <c r="C2" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>192</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="I2" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1331,17 +1370,17 @@
       <c r="C3" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="D3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="F3" t="s">
-        <v>217</v>
+      <c r="D3" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>226</v>
       </c>
       <c r="I3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1354,17 +1393,17 @@
       <c r="C4" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="D4" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="F4" t="s">
         <v>214</v>
       </c>
-      <c r="F4" t="s">
-        <v>218</v>
-      </c>
       <c r="I4" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="J4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1378,7 +1417,10 @@
         <v>196</v>
       </c>
       <c r="F5" t="s">
-        <v>220</v>
+        <v>215</v>
+      </c>
+      <c r="I5" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1389,7 +1431,13 @@
         <v>203</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>202</v>
+        <v>207</v>
+      </c>
+      <c r="F6" t="s">
+        <v>216</v>
+      </c>
+      <c r="I6" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1397,15 +1445,21 @@
         <v>195</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>208</v>
+        <v>202</v>
+      </c>
+      <c r="F7" t="s">
+        <v>227</v>
+      </c>
+      <c r="I7" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>226</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>206</v>
+        <v>222</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -1413,37 +1467,76 @@
         <v>197</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C10" s="10" t="s">
-        <v>207</v>
+        <v>235</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" s="10" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" s="10" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C13" s="10" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="10" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>227</v>
+        <v>239</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
group by/having/order by as separate nodes
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Uni\DataEngineering\WS22\Guided Research\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E67F1D2-B472-413A-9589-579B9E115F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5263A1DA-499E-40B9-B18E-8DC9FCE70945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19305" yWindow="1740" windowWidth="14325" windowHeight="11775" activeTab="1" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="38670" windowHeight="16470" activeTab="1" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
   <sheets>
     <sheet name="Meeting Notes" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="254">
   <si>
     <t>paper</t>
   </si>
@@ -643,9 +643,6 @@
     <t>expressions</t>
   </si>
   <si>
-    <t>case</t>
-  </si>
-  <si>
     <t>where</t>
   </si>
   <si>
@@ -770,6 +767,51 @@
   </si>
   <si>
     <t>TPCH Correlated</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t>date,interval,exists</t>
+  </si>
+  <si>
+    <t>in, double nested,date,interval</t>
+  </si>
+  <si>
+    <t>exists/not exists</t>
+  </si>
+  <si>
+    <t>in list,substring,not exists</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>detect correlated subquery without alias</t>
+  </si>
+  <si>
+    <t>schema</t>
+  </si>
+  <si>
+    <t>What makes Q2 harder than Q1? Same RA tree</t>
+  </si>
+  <si>
+    <t>group by as own operator</t>
+  </si>
+  <si>
+    <t>order by = sort operator (unter projection)</t>
+  </si>
+  <si>
+    <t>add step where scan whole query and map attributes to relations (for tpch)</t>
+  </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>having operator (like where)</t>
+  </si>
+  <si>
+    <t>case expression</t>
   </si>
 </sst>
 </file>
@@ -1282,13 +1324,13 @@
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>232</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -1299,15 +1341,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C36143C-8755-4841-9383-2CD561E91E02}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -1319,22 +1362,22 @@
         <v>191</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1342,7 +1385,7 @@
         <v>192</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>192</v>
@@ -1354,10 +1397,10 @@
         <v>192</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1368,19 +1411,17 @@
         <v>193</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>197</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="E3" s="13"/>
       <c r="F3" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1388,39 +1429,37 @@
         <v>194</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>197</v>
-      </c>
-      <c r="F4" t="s">
-        <v>214</v>
+        <v>204</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="F4" s="10" t="s">
+        <v>213</v>
       </c>
       <c r="I4" t="s">
+        <v>219</v>
+      </c>
+      <c r="J4" t="s">
         <v>220</v>
-      </c>
-      <c r="J4" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>196</v>
       </c>
       <c r="F5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1428,16 +1467,16 @@
         <v>196</v>
       </c>
       <c r="B6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="F6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1445,98 +1484,150 @@
         <v>195</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>223</v>
+      <c r="F8" t="s">
+        <v>246</v>
+      </c>
+      <c r="I8" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>197</v>
-      </c>
       <c r="C9" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
+      </c>
+      <c r="F9" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C10" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" s="10" t="s">
-        <v>208</v>
+        <v>207</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C13" s="10" t="s">
-        <v>212</v>
+        <v>211</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C14" s="10" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>244</v>
+      </c>
+      <c r="I15" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="B18" s="12" t="s">
         <v>239</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="D18" s="12" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>213</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>2</v>
-      </c>
-      <c r="C19" s="9" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>4</v>
+      </c>
+      <c r="B20" t="s">
+        <v>240</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>4</v>
-      </c>
-      <c r="C20" s="9" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="B22" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="B23" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
         <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>228</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exists/not exists, tpch 2,17,21, implicit group by
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Uni\DataEngineering\WS22\Guided Research\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5263A1DA-499E-40B9-B18E-8DC9FCE70945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B43B104-1520-4E47-A181-8F8A5A5E905E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-135" yWindow="-135" windowWidth="38670" windowHeight="16470" activeTab="1" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="270">
   <si>
     <t>paper</t>
   </si>
@@ -712,9 +712,6 @@
     <t>can integrate function evaluation (map and group by) into projection?</t>
   </si>
   <si>
-    <t>select min(id); select name+5</t>
-  </si>
-  <si>
     <t>agg functions (no group by)</t>
   </si>
   <si>
@@ -733,9 +730,6 @@
     <t>limit</t>
   </si>
   <si>
-    <t>can we assume we are working with sets?</t>
-  </si>
-  <si>
     <t>all</t>
   </si>
   <si>
@@ -751,9 +745,6 @@
     <t>Doesn't make sense to introduce dependent join in step 3, because then already decorrelated</t>
   </si>
   <si>
-    <t>exists (use DJ)</t>
-  </si>
-  <si>
     <t>in (use DJ)</t>
   </si>
   <si>
@@ -787,9 +778,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>detect correlated subquery without alias</t>
-  </si>
-  <si>
     <t>schema</t>
   </si>
   <si>
@@ -802,9 +790,6 @@
     <t>order by = sort operator (unter projection)</t>
   </si>
   <si>
-    <t>add step where scan whole query and map attributes to relations (for tpch)</t>
-  </si>
-  <si>
     <t>Todos</t>
   </si>
   <si>
@@ -812,6 +797,69 @@
   </si>
   <si>
     <t>case expression</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>expression</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>for us no big difference</t>
+  </si>
+  <si>
+    <t>Exist can be translated to dep left join. Can "in" always be translated into exists, then to dep left join?</t>
+  </si>
+  <si>
+    <t>Alex ask Neumann</t>
+  </si>
+  <si>
+    <t>Group by, order by, having as separate nodes</t>
+  </si>
+  <si>
+    <t>add step where scan whole query and map attributes to relations (for tpch), needed to detect if subquery is correlated</t>
+  </si>
+  <si>
+    <t>04.11.2022</t>
+  </si>
+  <si>
+    <t>Code review</t>
+  </si>
+  <si>
+    <t>Always treat exists as dep join</t>
+  </si>
+  <si>
+    <t>dependent join will fall away quickly in optimization?</t>
+  </si>
+  <si>
+    <t>clean up code</t>
+  </si>
+  <si>
+    <t>relational algebra .cc file</t>
+  </si>
+  <si>
+    <t>proper headers for .h files</t>
+  </si>
+  <si>
+    <t>initialize Ra Nodes properly</t>
+  </si>
+  <si>
+    <t>add implicit group by if aggregation func in select</t>
+  </si>
+  <si>
+    <t>detect tpch correlated subquery without alias</t>
+  </si>
+  <si>
+    <t>exists (SDJ)</t>
+  </si>
+  <si>
+    <t>not exists (ASDJ)</t>
+  </si>
+  <si>
+    <t>print greek characters</t>
   </si>
 </sst>
 </file>
@@ -887,7 +935,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -895,12 +943,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -923,6 +986,13 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1238,10 +1308,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FDCCB2-898C-4E8A-AEF1-A7FCAFD38A4A}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1324,13 +1394,47 @@
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>232</v>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="14" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>
@@ -1341,10 +1445,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C36143C-8755-4841-9383-2CD561E91E02}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,6 +1483,9 @@
       <c r="I1" s="8" t="s">
         <v>216</v>
       </c>
+      <c r="J1" s="8" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
@@ -1397,10 +1504,13 @@
         <v>192</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="I2" t="s">
+        <v>222</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>217</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1418,10 +1528,13 @@
       </c>
       <c r="E3" s="13"/>
       <c r="F3" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="I3" t="s">
+        <v>224</v>
+      </c>
+      <c r="I3" s="9" t="s">
         <v>218</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1438,11 +1551,11 @@
       <c r="F4" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="J4" t="s">
-        <v>220</v>
+      <c r="J4" s="9" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1458,8 +1571,11 @@
       <c r="F5" t="s">
         <v>214</v>
       </c>
-      <c r="I5" t="s">
-        <v>224</v>
+      <c r="I5" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1475,8 +1591,11 @@
       <c r="F6" t="s">
         <v>215</v>
       </c>
-      <c r="I6" t="s">
-        <v>227</v>
+      <c r="I6" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1487,147 +1606,164 @@
         <v>201</v>
       </c>
       <c r="F7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I7" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>222</v>
-      </c>
       <c r="F8" t="s">
-        <v>246</v>
-      </c>
-      <c r="I8" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C9" s="10" t="s">
-        <v>233</v>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="15" t="s">
+        <v>267</v>
       </c>
       <c r="F9" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C10" s="10" t="s">
-        <v>234</v>
+        <v>248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="15" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" s="10" t="s">
-        <v>207</v>
-      </c>
-      <c r="I12" s="9" t="s">
-        <v>248</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C13" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="I13" s="9" t="s">
-        <v>249</v>
+        <v>207</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C14" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>252</v>
+        <v>211</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="10" t="s">
+        <v>226</v>
+      </c>
       <c r="D15" t="s">
-        <v>244</v>
-      </c>
-      <c r="I15" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="6">
+        <v>232</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="16">
         <v>2</v>
       </c>
       <c r="B19" t="s">
         <v>213</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+        <v>234</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="16">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="I21" s="9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="6">
+        <v>238</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="J22" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="16">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>239</v>
+      </c>
+      <c r="J23" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+      <c r="J24" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>228</v>
-      </c>
-      <c r="B25" s="10" t="s">
-        <v>245</v>
+        <v>226</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>266</v>
+      </c>
+      <c r="I25" s="15" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I26" s="9" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
date, interval, tpch q4
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Uni\DataEngineering\WS22\Guided Research\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B43B104-1520-4E47-A181-8F8A5A5E905E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E01BC4-029B-4C9F-99F0-708AB2175236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-135" yWindow="-135" windowWidth="38670" windowHeight="16470" activeTab="1" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
@@ -935,7 +935,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -958,12 +958,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -991,6 +1028,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1448,14 +1491,14 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
@@ -1641,18 +1684,18 @@
         <v>231</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="10" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C13" s="10" t="s">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="15" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C14" s="10" t="s">
+    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C14" s="15" t="s">
         <v>211</v>
       </c>
     </row>
@@ -1664,7 +1707,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>235</v>
       </c>
@@ -1678,7 +1721,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16">
         <v>2</v>
       </c>
@@ -1688,12 +1731,12 @@
       <c r="D19" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="I19" s="9" t="s">
+      <c r="I19" s="17" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
+    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="20">
         <v>4</v>
       </c>
       <c r="B20" t="s">
@@ -1702,15 +1745,15 @@
       <c r="D20" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="I20" s="9" t="s">
+      <c r="I20" s="18" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16">
         <v>17</v>
       </c>
-      <c r="I21" s="9" t="s">
+      <c r="I21" s="19" t="s">
         <v>247</v>
       </c>
     </row>

</xml_diff>

<commit_message>
parse tpch, all but in keyword
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Uni\DataEngineering\WS22\Guided Research\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E01BC4-029B-4C9F-99F0-708AB2175236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473ED461-4F31-485D-8CA5-D9EE0DD4A457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="38670" windowHeight="16470" activeTab="1" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" activeTab="1" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
   <sheets>
     <sheet name="Meeting Notes" sheetId="4" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Optimizers" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="282">
   <si>
     <t>paper</t>
   </si>
@@ -658,9 +659,6 @@
     <t>subqueries</t>
   </si>
   <si>
-    <t>joins</t>
-  </si>
-  <si>
     <t>consts</t>
   </si>
   <si>
@@ -691,12 +689,12 @@
     <t>general</t>
   </si>
   <si>
-    <t>like</t>
-  </si>
-  <si>
     <t>views</t>
   </si>
   <si>
+    <t>in</t>
+  </si>
+  <si>
     <t>substring</t>
   </si>
   <si>
@@ -763,24 +761,12 @@
     <t>missing</t>
   </si>
   <si>
-    <t>date,interval,exists</t>
-  </si>
-  <si>
-    <t>in, double nested,date,interval</t>
-  </si>
-  <si>
-    <t>exists/not exists</t>
-  </si>
-  <si>
-    <t>in list,substring,not exists</t>
+    <t>in, double nested</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>schema</t>
-  </si>
-  <si>
     <t>What makes Q2 harder than Q1? Same RA tree</t>
   </si>
   <si>
@@ -860,6 +846,57 @@
   </si>
   <si>
     <t>print greek characters</t>
+  </si>
+  <si>
+    <t>in list</t>
+  </si>
+  <si>
+    <t>namespace around funcs</t>
+  </si>
+  <si>
+    <t>TPCH Other</t>
+  </si>
+  <si>
+    <t>expression parenthesis</t>
+  </si>
+  <si>
+    <t>16 (is correlated??)</t>
+  </si>
+  <si>
+    <t>18 (is correlated??)</t>
+  </si>
+  <si>
+    <t>19 (is correlated??)</t>
+  </si>
+  <si>
+    <t>debug print everything</t>
+  </si>
+  <si>
+    <t>like/not like</t>
+  </si>
+  <si>
+    <t>distinct</t>
+  </si>
+  <si>
+    <t>in, not in</t>
+  </si>
+  <si>
+    <t>extract</t>
+  </si>
+  <si>
+    <t>left outer join</t>
+  </si>
+  <si>
+    <t>deconstructor deletes</t>
+  </si>
+  <si>
+    <t>using (join)</t>
+  </si>
+  <si>
+    <t>natural (join)</t>
+  </si>
+  <si>
+    <t>table schema</t>
   </si>
 </sst>
 </file>
@@ -897,7 +934,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -928,14 +965,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -958,49 +989,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1020,9 +1014,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1030,12 +1023,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1437,47 +1425,47 @@
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>229</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
         <v>255</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="13" t="s">
+        <v>250</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -1488,10 +1476,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C36143C-8755-4841-9383-2CD561E91E02}">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1515,19 +1503,19 @@
         <v>197</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1547,13 +1535,13 @@
         <v>192</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1564,23 +1552,22 @@
         <v>193</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="E3" s="13"/>
+        <v>208</v>
+      </c>
       <c r="F3" s="9" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>194</v>
       </c>
@@ -1588,226 +1575,331 @@
         <v>200</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="D4" s="13"/>
-      <c r="F4" s="10" t="s">
-        <v>213</v>
+        <v>203</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>273</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="B5" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>201</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="F5" t="s">
-        <v>214</v>
+      <c r="F5" s="14" t="s">
+        <v>212</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="B6" t="s">
-        <v>202</v>
+      <c r="B6" s="14" t="s">
+        <v>277</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>206</v>
-      </c>
-      <c r="F6" t="s">
-        <v>215</v>
+        <v>205</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>214</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>195</v>
       </c>
+      <c r="B7" t="s">
+        <v>220</v>
+      </c>
       <c r="C7" s="9" t="s">
         <v>201</v>
       </c>
       <c r="F7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" t="s">
+        <v>279</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>221</v>
-      </c>
       <c r="F8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="F11" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="D15" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>234</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>267</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
+        <v>2</v>
+      </c>
+      <c r="C21" s="15">
+        <v>1</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
+        <v>4</v>
+      </c>
+      <c r="C22" s="15">
+        <v>3</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
+        <v>17</v>
+      </c>
+      <c r="C23" s="15">
+        <v>5</v>
+      </c>
+      <c r="I23" s="9" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="F9" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="15" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C11" s="10" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="10" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="15" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="15" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="D15" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
-        <v>235</v>
-      </c>
-      <c r="B18" s="12" t="s">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
         <v>236</v>
       </c>
-      <c r="D18" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16">
-        <v>2</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="C24" s="15">
+        <v>6</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="15">
+        <v>21</v>
+      </c>
+      <c r="C25" s="15">
+        <v>7</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>265</v>
+      </c>
+      <c r="C26" s="15">
+        <v>8</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="J26" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>225</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="C27" s="15">
+        <v>9</v>
+      </c>
+      <c r="J27" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C28" s="15">
+        <v>10</v>
+      </c>
+      <c r="J28" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C29" s="15">
+        <v>11</v>
+      </c>
+      <c r="J29" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C30" s="6">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
         <v>213</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="I19" s="17" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="20">
-        <v>4</v>
-      </c>
-      <c r="B20" t="s">
-        <v>237</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="I20" s="18" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="16">
-        <v>17</v>
-      </c>
-      <c r="I21" s="19" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>238</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="J22" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="16">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>239</v>
-      </c>
-      <c r="J23" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="6">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>240</v>
-      </c>
-      <c r="J24" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>226</v>
-      </c>
-      <c r="B25" s="15" t="s">
-        <v>266</v>
-      </c>
-      <c r="I25" s="15" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I26" s="9" t="s">
+      <c r="J30" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="6" t="s">
         <v>269</v>
       </c>
+      <c r="D34" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="D35" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="D36" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C37" s="6"/>
+    </row>
+    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C38" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cleanup and refactor code
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Uni\DataEngineering\WS22\Guided Research\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473ED461-4F31-485D-8CA5-D9EE0DD4A457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FD4596-AD19-4DB4-88B5-516334C5D20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" activeTab="1" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="284">
   <si>
     <t>paper</t>
   </si>
@@ -692,24 +692,12 @@
     <t>views</t>
   </si>
   <si>
-    <t>in</t>
-  </si>
-  <si>
     <t>substring</t>
   </si>
   <si>
     <t>questions</t>
   </si>
   <si>
-    <t>case when… to RA?</t>
-  </si>
-  <si>
-    <t>is RA rename operator needed? Just integrate into projection</t>
-  </si>
-  <si>
-    <t>can integrate function evaluation (map and group by) into projection?</t>
-  </si>
-  <si>
     <t>agg functions (no group by)</t>
   </si>
   <si>
@@ -719,9 +707,6 @@
     <t>print RA tree</t>
   </si>
   <si>
-    <t>can integrate group/order by into projection?</t>
-  </si>
-  <si>
     <t>(-) column ref</t>
   </si>
   <si>
@@ -767,9 +752,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>What makes Q2 harder than Q1? Same RA tree</t>
-  </si>
-  <si>
     <t>group by as own operator</t>
   </si>
   <si>
@@ -788,15 +770,6 @@
     <t>answer</t>
   </si>
   <si>
-    <t>expression</t>
-  </si>
-  <si>
-    <t>ok</t>
-  </si>
-  <si>
-    <t>for us no big difference</t>
-  </si>
-  <si>
     <t>Exist can be translated to dep left join. Can "in" always be translated into exists, then to dep left join?</t>
   </si>
   <si>
@@ -851,9 +824,6 @@
     <t>in list</t>
   </si>
   <si>
-    <t>namespace around funcs</t>
-  </si>
-  <si>
     <t>TPCH Other</t>
   </si>
   <si>
@@ -897,6 +867,43 @@
   </si>
   <si>
     <t>table schema</t>
+  </si>
+  <si>
+    <t>funcs into classes</t>
+  </si>
+  <si>
+    <t>12 (is correlated??)</t>
+  </si>
+  <si>
+    <t>print indentation</t>
+  </si>
+  <si>
+    <t>print correlated joins</t>
+  </si>
+  <si>
+    <t>add ' to date cast</t>
+  </si>
+  <si>
+    <t>optimize CTEs separately</t>
+  </si>
+  <si>
+    <t>smart pointer &gt; C pointer
+Keep code recursive rather than iterative for less complexity</t>
+  </si>
+  <si>
+    <t>translate "in" to "exists" + null check</t>
+  </si>
+  <si>
+    <t>side effect: uncorrelated "in" queries will become correlated</t>
+  </si>
+  <si>
+    <t>Don't integrate CTEs into the main RA tree, but optimize and keep them separately</t>
+  </si>
+  <si>
+    <t>translate in to exists</t>
+  </si>
+  <si>
+    <t>deparse dependent joins</t>
   </si>
 </sst>
 </file>
@@ -994,7 +1001,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1015,7 +1022,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1024,6 +1030,8 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1339,10 +1347,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FDCCB2-898C-4E8A-AEF1-A7FCAFD38A4A}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,47 +1433,63 @@
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
-        <v>250</v>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>253</v>
+        <v>244</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -1478,14 +1502,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C36143C-8755-4841-9383-2CD561E91E02}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
@@ -1512,10 +1536,10 @@
         <v>211</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1535,13 +1559,10 @@
         <v>192</v>
       </c>
       <c r="F2" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="I2" t="s">
         <v>221</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>216</v>
-      </c>
-      <c r="J2" s="9" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1558,14 +1579,10 @@
         <v>208</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="I3" s="9" t="s">
-        <v>217</v>
-      </c>
-      <c r="J3" s="9" t="s">
-        <v>246</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
@@ -1578,199 +1595,193 @@
         <v>203</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>246</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>201</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="I5" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>9</v>
-      </c>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>277</v>
+      <c r="B6" s="13" t="s">
+        <v>267</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>205</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="I6" s="9" t="s">
-        <v>238</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>247</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="I6" s="16"/>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>195</v>
       </c>
       <c r="B7" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>201</v>
       </c>
       <c r="F7" t="s">
-        <v>224</v>
-      </c>
-      <c r="I7" t="s">
-        <v>226</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="I7" s="17"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="B8" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F8" t="s">
-        <v>281</v>
-      </c>
+        <v>271</v>
+      </c>
+      <c r="I8" s="16"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>243</v>
-      </c>
+        <v>253</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="I9" s="17"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10" s="9" t="s">
-        <v>263</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>268</v>
+        <v>254</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="10" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F11" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>204</v>
       </c>
-      <c r="F12" s="14" t="s">
-        <v>274</v>
+      <c r="F12" s="13" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="F13" s="14" t="s">
-        <v>276</v>
+      <c r="F13" s="13" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C14" s="9" t="s">
         <v>210</v>
       </c>
+      <c r="F14" s="16" t="s">
+        <v>274</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="16" t="s">
-        <v>225</v>
+      <c r="C15" s="15" t="s">
+        <v>220</v>
       </c>
       <c r="D15" t="s">
-        <v>237</v>
+        <v>232</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="14">
+        <v>2</v>
+      </c>
+      <c r="C21" s="14">
+        <v>1</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="14">
+        <v>4</v>
+      </c>
+      <c r="C22" s="14">
+        <v>3</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="I22" s="9" t="s">
         <v>234</v>
       </c>
-      <c r="B20" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>235</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>231</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="15">
-        <v>2</v>
-      </c>
-      <c r="C21" s="15">
-        <v>1</v>
-      </c>
-      <c r="E21" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="I21" s="9" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="15">
-        <v>4</v>
-      </c>
-      <c r="C22" s="15">
-        <v>3</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>240</v>
-      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="15">
+      <c r="A23" s="14">
         <v>17</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="14">
         <v>5</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -1778,24 +1789,24 @@
         <v>20</v>
       </c>
       <c r="B24" t="s">
-        <v>236</v>
-      </c>
-      <c r="C24" s="15">
+        <v>231</v>
+      </c>
+      <c r="C24" s="14">
         <v>6</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="15">
+      <c r="A25" s="14">
         <v>21</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="14">
         <v>7</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1803,102 +1814,114 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>265</v>
-      </c>
-      <c r="C26" s="15">
+        <v>256</v>
+      </c>
+      <c r="C26" s="14">
         <v>8</v>
       </c>
-      <c r="I26" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="J26" t="s">
-        <v>257</v>
+      <c r="I26" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C27" s="14">
+        <v>9</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C28" s="14">
+        <v>10</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C29" s="14">
+        <v>11</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C30" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="D30" t="s">
+        <v>256</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="14">
+        <v>13</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="14">
+        <v>14</v>
+      </c>
+      <c r="I32" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="14">
+        <v>15</v>
+      </c>
+      <c r="I33" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="D34" t="s">
+        <v>265</v>
+      </c>
+      <c r="I34" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C35" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D35" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C36" s="6" t="s">
         <v>261</v>
       </c>
-      <c r="C27" s="15">
-        <v>9</v>
-      </c>
-      <c r="J27" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C28" s="15">
-        <v>10</v>
-      </c>
-      <c r="J28" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C29" s="15">
-        <v>11</v>
-      </c>
-      <c r="J29" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C30" s="6">
-        <v>12</v>
-      </c>
-      <c r="D30" t="s">
-        <v>213</v>
-      </c>
-      <c r="J30" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C31" s="15">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C32" s="15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="15">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="6" t="s">
-        <v>269</v>
-      </c>
-      <c r="D34" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="D35" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="6" t="s">
-        <v>271</v>
-      </c>
       <c r="D36" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" s="6"/>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="6"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
keep CTEs and parse/optimize/deparse them separately
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Uni\DataEngineering\WS22\Guided Research\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FD4596-AD19-4DB4-88B5-516334C5D20A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F27134-10BC-4D6B-9EDB-9565DF17A5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" activeTab="1" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="286">
   <si>
     <t>paper</t>
   </si>
@@ -875,9 +875,6 @@
     <t>12 (is correlated??)</t>
   </si>
   <si>
-    <t>print indentation</t>
-  </si>
-  <si>
     <t>print correlated joins</t>
   </si>
   <si>
@@ -904,6 +901,15 @@
   </si>
   <si>
     <t>deparse dependent joins</t>
+  </si>
+  <si>
+    <t>pretty print</t>
+  </si>
+  <si>
+    <t>tests</t>
+  </si>
+  <si>
+    <t>new RATree class (root, ctes, relation schemas)</t>
   </si>
 </sst>
 </file>
@@ -1476,20 +1482,20 @@
         <v>244</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>279</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -1503,7 +1509,7 @@
   <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1711,7 +1717,7 @@
         <v>210</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1722,7 +1728,12 @@
         <v>232</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>275</v>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F16" s="16" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -1872,15 +1883,18 @@
         <v>13</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C32" s="14">
         <v>14</v>
       </c>
-      <c r="I32" t="s">
-        <v>277</v>
+      <c r="I32" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
@@ -1888,7 +1902,7 @@
         <v>15</v>
       </c>
       <c r="I33" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="34" spans="3:9" x14ac:dyDescent="0.25">
@@ -1899,7 +1913,7 @@
         <v>265</v>
       </c>
       <c r="I34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="35" spans="3:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
parse in clause, null check
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Uni\DataEngineering\WS22\Guided Research\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F27134-10BC-4D6B-9EDB-9565DF17A5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A26DD4E-5724-4B02-B408-E35F15E3EB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="16440" activeTab="1" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
+    <workbookView xWindow="0" yWindow="1740" windowWidth="9495" windowHeight="11775" activeTab="1" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
   <sheets>
     <sheet name="Meeting Notes" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="286">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="285">
   <si>
     <t>paper</t>
   </si>
@@ -692,6 +692,9 @@
     <t>views</t>
   </si>
   <si>
+    <t>in</t>
+  </si>
+  <si>
     <t>substring</t>
   </si>
   <si>
@@ -746,9 +749,6 @@
     <t>missing</t>
   </si>
   <si>
-    <t>in, double nested</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -830,15 +830,6 @@
     <t>expression parenthesis</t>
   </si>
   <si>
-    <t>16 (is correlated??)</t>
-  </si>
-  <si>
-    <t>18 (is correlated??)</t>
-  </si>
-  <si>
-    <t>19 (is correlated??)</t>
-  </si>
-  <si>
     <t>debug print everything</t>
   </si>
   <si>
@@ -870,9 +861,6 @@
   </si>
   <si>
     <t>funcs into classes</t>
-  </si>
-  <si>
-    <t>12 (is correlated??)</t>
   </si>
   <si>
     <t>print correlated joins</t>
@@ -910,6 +898,15 @@
   </si>
   <si>
     <t>new RATree class (root, ctes, relation schemas)</t>
+  </si>
+  <si>
+    <t>translate in list to in subquery</t>
+  </si>
+  <si>
+    <t>add null check for in</t>
+  </si>
+  <si>
+    <t>is null/is not null</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1004,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1036,8 +1033,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1439,13 +1440,13 @@
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1482,20 +1483,20 @@
         <v>244</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
   </sheetData>
@@ -1508,8 +1509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C36143C-8755-4841-9383-2CD561E91E02}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1542,7 +1543,7 @@
         <v>211</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J1" s="8" t="s">
         <v>238</v>
@@ -1565,10 +1566,10 @@
         <v>192</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="I2" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1585,12 +1586,12 @@
         <v>208</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
     </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>194</v>
       </c>
@@ -1601,41 +1602,41 @@
         <v>203</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="16" t="s">
         <v>201</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="16" t="s">
         <v>212</v>
       </c>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>267</v>
+      <c r="B6" s="16" t="s">
+        <v>264</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>205</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="I6" s="16"/>
+        <v>214</v>
+      </c>
+      <c r="I6" s="17"/>
       <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1643,114 +1644,117 @@
         <v>195</v>
       </c>
       <c r="B7" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>201</v>
       </c>
       <c r="F7" t="s">
-        <v>219</v>
-      </c>
-      <c r="I7" s="17"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+      <c r="I7" s="18"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B8" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F8" t="s">
-        <v>271</v>
-      </c>
-      <c r="I8" s="16"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>268</v>
+      </c>
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="16" t="s">
         <v>237</v>
       </c>
-      <c r="I9" s="17"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="18"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C10" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="16" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="10" t="s">
-        <v>225</v>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="9" t="s">
+        <v>226</v>
       </c>
       <c r="F11" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="13" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="16" t="s">
         <v>204</v>
       </c>
-      <c r="F12" s="13" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F12" s="16" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C13" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="F13" s="13" t="s">
-        <v>266</v>
+      <c r="F13" s="16" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C14" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="F14" s="16" t="s">
-        <v>283</v>
+      <c r="F14" s="17" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C15" s="15" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="D15" t="s">
         <v>232</v>
       </c>
-      <c r="F15" s="16" t="s">
-        <v>274</v>
+      <c r="F15" s="17" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F16" s="16" t="s">
+      <c r="C16" s="9" t="s">
         <v>284</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C20" s="11" t="s">
         <v>257</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="I20" s="8" t="s">
         <v>235</v>
@@ -1764,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="I21" s="9" t="s">
         <v>233</v>
@@ -1778,15 +1782,18 @@
         <v>3</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="I22" s="9" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="14">
-        <v>17</v>
+      <c r="A23" s="19">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>256</v>
       </c>
       <c r="C23" s="14">
         <v>5</v>
@@ -1796,11 +1803,11 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="6">
-        <v>20</v>
+      <c r="A24" s="19">
+        <v>16</v>
       </c>
       <c r="B24" t="s">
-        <v>231</v>
+        <v>262</v>
       </c>
       <c r="C24" s="14">
         <v>6</v>
@@ -1809,9 +1816,9 @@
         <v>251</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="14">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C25" s="14">
         <v>7</v>
@@ -1820,9 +1827,9 @@
         <v>255</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="6">
-        <v>22</v>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="19">
+        <v>18</v>
       </c>
       <c r="B26" t="s">
         <v>256</v>
@@ -1830,7 +1837,7 @@
       <c r="C26" s="14">
         <v>8</v>
       </c>
-      <c r="I26" s="13" t="s">
+      <c r="I26" s="16" t="s">
         <v>247</v>
       </c>
       <c r="J26" s="9" t="s">
@@ -1838,11 +1845,11 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>220</v>
-      </c>
-      <c r="B27" s="9" t="s">
-        <v>252</v>
+      <c r="A27" s="19">
+        <v>19</v>
+      </c>
+      <c r="B27" t="s">
+        <v>256</v>
       </c>
       <c r="C27" s="14">
         <v>9</v>
@@ -1852,6 +1859,12 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="19">
+        <v>20</v>
+      </c>
+      <c r="B28" t="s">
+        <v>213</v>
+      </c>
       <c r="C28" s="14">
         <v>10</v>
       </c>
@@ -1860,80 +1873,78 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="14">
+        <v>21</v>
+      </c>
       <c r="C29" s="14">
         <v>11</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C30" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="D30" t="s">
+      <c r="A30" s="19">
+        <v>22</v>
+      </c>
+      <c r="B30" t="s">
         <v>256</v>
       </c>
+      <c r="C30" s="14">
+        <v>13</v>
+      </c>
       <c r="J30" s="9" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>221</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>252</v>
+      </c>
       <c r="C31" s="14">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C32" s="14">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="J32" s="9" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C33" s="14">
-        <v>15</v>
-      </c>
-      <c r="I33" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C34" s="6" t="s">
-        <v>259</v>
-      </c>
-      <c r="D34" t="s">
-        <v>265</v>
-      </c>
-      <c r="I34" t="s">
+      <c r="I33" s="9" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I34" s="9" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C35" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="D35" t="s">
-        <v>256</v>
+    <row r="35" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I35" s="13" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="36" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C36" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="D36" t="s">
-        <v>256</v>
+      <c r="I36" s="10" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" s="6"/>
+      <c r="I37" s="15"/>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C38" s="6"/>

</xml_diff>

<commit_message>
parse in list as predicate, parse tpch 19
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Uni\DataEngineering\WS22\Guided Research\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A26DD4E-5724-4B02-B408-E35F15E3EB27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6ACE8787-15F0-4FD1-A191-A5D60386370D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1740" windowWidth="9495" windowHeight="11775" activeTab="1" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
+    <workbookView xWindow="0" yWindow="1740" windowWidth="21630" windowHeight="13455" activeTab="2" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
   <sheets>
     <sheet name="Meeting Notes" sheetId="4" r:id="rId1"/>
-    <sheet name="SQL Parser" sheetId="5" r:id="rId2"/>
-    <sheet name="Papers" sheetId="1" r:id="rId3"/>
-    <sheet name="Parsers" sheetId="2" r:id="rId4"/>
-    <sheet name="Optimizers" sheetId="3" r:id="rId5"/>
+    <sheet name="inexists" sheetId="6" r:id="rId2"/>
+    <sheet name="SQL Parser" sheetId="5" r:id="rId3"/>
+    <sheet name="Papers" sheetId="1" r:id="rId4"/>
+    <sheet name="Parsers" sheetId="2" r:id="rId5"/>
+    <sheet name="Optimizers" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="324">
   <si>
     <t>paper</t>
   </si>
@@ -821,9 +822,6 @@
     <t>print greek characters</t>
   </si>
   <si>
-    <t>in list</t>
-  </si>
-  <si>
     <t>TPCH Other</t>
   </si>
   <si>
@@ -837,9 +835,6 @@
   </si>
   <si>
     <t>distinct</t>
-  </si>
-  <si>
-    <t>in, not in</t>
   </si>
   <si>
     <t>extract</t>
@@ -907,6 +902,129 @@
   </si>
   <si>
     <t>is null/is not null</t>
+  </si>
+  <si>
+    <t>group by needs extra arg, would make RA tree invalid</t>
+  </si>
+  <si>
+    <t>use left joins by default</t>
+  </si>
+  <si>
+    <t>why div by 0 error in umbra</t>
+  </si>
+  <si>
+    <t>08.11.2022</t>
+  </si>
+  <si>
+    <t>sql has no semi join or anti join</t>
+  </si>
+  <si>
+    <t>to decorrelate "in" and "exists", need to transform semi joins to regular joins</t>
+  </si>
+  <si>
+    <t>deparsing exists/in</t>
+  </si>
+  <si>
+    <t>exists predicate needs to stay in selection, with a marker</t>
+  </si>
+  <si>
+    <t>in values -&gt; store in predicate, not subquery</t>
+  </si>
+  <si>
+    <t>introduce special join for in subquery (how are correlated in subqueries decorrelated?)</t>
+  </si>
+  <si>
+    <t>translate exists to cp, doesn't work for not exists?</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>exists</t>
+  </si>
+  <si>
+    <t>not exists</t>
+  </si>
+  <si>
+    <t>not in</t>
+  </si>
+  <si>
+    <t>input</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>correlated exists subquery</t>
+  </si>
+  <si>
+    <t>summary</t>
+  </si>
+  <si>
+    <t>only eq predicates</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>uncorrelated subquery</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>not exists unnested to left join where is null</t>
+  </si>
+  <si>
+    <t>select * from students s where exists (select a.studnr from attend a where a.studnr=26120);</t>
+  </si>
+  <si>
+    <t>select s.* from students s left join (select distinct studnr from attend) a on a.studnr=26120 where a.studnr is not null;</t>
+  </si>
+  <si>
+    <t>select * from students s where not exists (select studnr from attend where studnr=24002);</t>
+  </si>
+  <si>
+    <t>select s.* from students s left join attend a on a.studnr=24002 where a.studnr is null;</t>
+  </si>
+  <si>
+    <t>select s.* from students s left join (select distinct studnr from attend) a on a.studnr=s.studnr where a.studnr is not null;</t>
+  </si>
+  <si>
+    <t>select * from students s where exists (select a.studnr from attend a where a.studnr=s.studnr);</t>
+  </si>
+  <si>
+    <t>exists unnested to left join (select distinct) where is not null; only for eq</t>
+  </si>
+  <si>
+    <t>same as above, only for eq</t>
+  </si>
+  <si>
+    <t>focus on eq subquery connections</t>
+  </si>
+  <si>
+    <t>do we only decorrelate, or also unnest in general</t>
+  </si>
+  <si>
+    <t>change in list to simple predicate</t>
   </si>
 </sst>
 </file>
@@ -976,7 +1094,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -999,12 +1117,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1023,7 +1150,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1032,13 +1158,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1354,10 +1479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FDCCB2-898C-4E8A-AEF1-A7FCAFD38A4A}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,7 +1490,8 @@
     <col min="1" max="1" width="24.140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="55.5703125" style="4" customWidth="1"/>
     <col min="3" max="3" width="65.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="4"/>
+    <col min="4" max="4" width="30.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1465,8 +1591,8 @@
         <v>246</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
+    <row r="12" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="11" t="s">
         <v>241</v>
       </c>
     </row>
@@ -1483,20 +1609,54 @@
         <v>244</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C19" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="4" t="s">
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -1506,11 +1666,162 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E917740-AD23-492A-8962-EF2BCDE6AB5A}">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C1" t="s">
+        <v>298</v>
+      </c>
+      <c r="D1" t="s">
+        <v>299</v>
+      </c>
+      <c r="E1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="B2" t="s">
+        <v>309</v>
+      </c>
+      <c r="C2" t="s">
+        <v>313</v>
+      </c>
+      <c r="D2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C3" t="s">
+        <v>318</v>
+      </c>
+      <c r="D3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="B4" t="s">
+        <v>309</v>
+      </c>
+      <c r="C4" t="s">
+        <v>315</v>
+      </c>
+      <c r="D4" t="s">
+        <v>316</v>
+      </c>
+      <c r="E4" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>310</v>
+      </c>
+      <c r="H14" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>305</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>303</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>321</v>
+      </c>
+      <c r="G16" t="s">
+        <v>306</v>
+      </c>
+      <c r="H16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>295</v>
+      </c>
+      <c r="B17" t="s">
+        <v>304</v>
+      </c>
+      <c r="G17" t="s">
+        <v>307</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>322</v>
+      </c>
+      <c r="G18" t="s">
+        <v>308</v>
+      </c>
+      <c r="H18">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C36143C-8755-4841-9383-2CD561E91E02}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,8 +1899,6 @@
       <c r="F3" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
@@ -1602,33 +1911,29 @@
         <v>203</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
+        <v>259</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="9" t="s">
         <v>201</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>264</v>
+      <c r="B6" s="9" t="s">
+        <v>262</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>205</v>
@@ -1636,8 +1941,6 @@
       <c r="F6" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
@@ -1652,41 +1955,38 @@
       <c r="F7" t="s">
         <v>220</v>
       </c>
-      <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>216</v>
       </c>
       <c r="B8" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>217</v>
       </c>
       <c r="F8" t="s">
-        <v>268</v>
-      </c>
-      <c r="I8" s="17"/>
+        <v>266</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C10" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="F10" s="16" t="s">
-        <v>258</v>
+      <c r="F10" s="9" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -1694,66 +1994,66 @@
         <v>226</v>
       </c>
       <c r="F11" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="F12" s="16" t="s">
-        <v>261</v>
+      <c r="F12" s="9" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C13" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="F13" s="16" t="s">
-        <v>263</v>
+      <c r="F13" s="9" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C14" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="F14" s="17" t="s">
-        <v>279</v>
+      <c r="F14" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C15" s="15" t="s">
+      <c r="C15" t="s">
         <v>221</v>
       </c>
       <c r="D15" t="s">
         <v>232</v>
       </c>
-      <c r="F15" s="17" t="s">
-        <v>270</v>
+      <c r="F15" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C16" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>280</v>
+        <v>282</v>
+      </c>
+      <c r="F16" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="B20" s="11" t="s">
+      <c r="B20" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="D20" s="11" t="s">
+      <c r="C20" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="D20" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="10" t="s">
         <v>227</v>
       </c>
       <c r="I20" s="8" t="s">
@@ -1761,10 +2061,10 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
+      <c r="A21" s="13">
         <v>2</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="13">
         <v>1</v>
       </c>
       <c r="E21" s="9" t="s">
@@ -1775,10 +2075,10 @@
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="14">
+      <c r="A22" s="13">
         <v>4</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="13">
         <v>3</v>
       </c>
       <c r="E22" s="9" t="s">
@@ -1789,13 +2089,10 @@
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="19">
+      <c r="A23" s="13">
         <v>12</v>
       </c>
-      <c r="B23" t="s">
-        <v>256</v>
-      </c>
-      <c r="C23" s="14">
+      <c r="C23" s="13">
         <v>5</v>
       </c>
       <c r="I23" s="9" t="s">
@@ -1803,13 +2100,10 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="19">
+      <c r="A24" s="13">
         <v>16</v>
       </c>
-      <c r="B24" t="s">
-        <v>262</v>
-      </c>
-      <c r="C24" s="14">
+      <c r="C24" s="13">
         <v>6</v>
       </c>
       <c r="I24" s="9" t="s">
@@ -1817,10 +2111,13 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="14">
+      <c r="A25" s="13">
         <v>17</v>
       </c>
-      <c r="C25" s="14">
+      <c r="B25" t="s">
+        <v>285</v>
+      </c>
+      <c r="C25" s="13">
         <v>7</v>
       </c>
       <c r="I25" s="9" t="s">
@@ -1828,16 +2125,13 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="19">
+      <c r="A26" s="13">
         <v>18</v>
       </c>
-      <c r="B26" t="s">
-        <v>256</v>
-      </c>
-      <c r="C26" s="14">
+      <c r="C26" s="13">
         <v>8</v>
       </c>
-      <c r="I26" s="16" t="s">
+      <c r="I26" s="9" t="s">
         <v>247</v>
       </c>
       <c r="J26" s="9" t="s">
@@ -1845,13 +2139,10 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="19">
+      <c r="A27" s="13">
         <v>19</v>
       </c>
-      <c r="B27" t="s">
-        <v>256</v>
-      </c>
-      <c r="C27" s="14">
+      <c r="C27" s="13">
         <v>9</v>
       </c>
       <c r="J27" s="9" t="s">
@@ -1859,13 +2150,10 @@
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="19">
+      <c r="A28" s="13">
         <v>20</v>
       </c>
-      <c r="B28" t="s">
-        <v>213</v>
-      </c>
-      <c r="C28" s="14">
+      <c r="C28" s="13">
         <v>10</v>
       </c>
       <c r="J28" s="9" t="s">
@@ -1873,28 +2161,28 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="14">
+      <c r="A29" s="13">
         <v>21</v>
       </c>
       <c r="C29" s="14">
         <v>11</v>
       </c>
+      <c r="D29" t="s">
+        <v>283</v>
+      </c>
       <c r="J29" s="9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="19">
+      <c r="A30" s="13">
         <v>22</v>
       </c>
-      <c r="B30" t="s">
-        <v>256</v>
-      </c>
-      <c r="C30" s="14">
+      <c r="C30" s="13">
         <v>13</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
@@ -1904,49 +2192,54 @@
       <c r="B31" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="13">
         <v>14</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C32" s="14">
+      <c r="C32" s="13">
         <v>15</v>
       </c>
       <c r="I32" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="J32" s="9" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I33" s="9" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I34" s="9" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I35" s="9" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="I33" s="9" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="34" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I34" s="9" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="35" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I35" s="13" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="I36" s="10" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I36" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="J36" s="9" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C37" s="6"/>
-      <c r="I37" s="15"/>
-    </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I37" s="17" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C38" s="6"/>
     </row>
   </sheetData>
@@ -1955,7 +2248,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C530AA-EE6D-4730-B7FC-66C1C2338D8E}">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -2358,7 +2651,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800A685A-9F16-4D2A-89B8-E0E1402FCD61}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -2726,7 +3019,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D31B28C7-0856-B849-8670-D0B5AB075FAE}">
   <dimension ref="A1:E5"/>
   <sheetViews>

</xml_diff>

<commit_message>
decorrelate simply correlated exists to in
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Uni\DataEngineering\WS22\Guided Research\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6ACE8787-15F0-4FD1-A191-A5D60386370D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDB5949-6407-44DE-A728-2BF0A121B2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1740" windowWidth="21630" windowHeight="13455" activeTab="2" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
+    <workbookView xWindow="2460" yWindow="255" windowWidth="22140" windowHeight="15165" activeTab="1" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
   <sheets>
     <sheet name="Meeting Notes" sheetId="4" r:id="rId1"/>
-    <sheet name="inexists" sheetId="6" r:id="rId2"/>
+    <sheet name="Tests" sheetId="6" r:id="rId2"/>
     <sheet name="SQL Parser" sheetId="5" r:id="rId3"/>
-    <sheet name="Papers" sheetId="1" r:id="rId4"/>
-    <sheet name="Parsers" sheetId="2" r:id="rId5"/>
-    <sheet name="Optimizers" sheetId="3" r:id="rId6"/>
+    <sheet name="RA optimizer" sheetId="7" r:id="rId4"/>
+    <sheet name="Papers" sheetId="1" r:id="rId5"/>
+    <sheet name="Parsers" sheetId="2" r:id="rId6"/>
+    <sheet name="Optimizers" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="307">
   <si>
     <t>paper</t>
   </si>
@@ -693,9 +694,6 @@
     <t>views</t>
   </si>
   <si>
-    <t>in</t>
-  </si>
-  <si>
     <t>substring</t>
   </si>
   <si>
@@ -904,15 +902,9 @@
     <t>is null/is not null</t>
   </si>
   <si>
-    <t>group by needs extra arg, would make RA tree invalid</t>
-  </si>
-  <si>
     <t>use left joins by default</t>
   </si>
   <si>
-    <t>why div by 0 error in umbra</t>
-  </si>
-  <si>
     <t>08.11.2022</t>
   </si>
   <si>
@@ -937,94 +929,52 @@
     <t>translate exists to cp, doesn't work for not exists?</t>
   </si>
   <si>
-    <t>Case</t>
-  </si>
-  <si>
-    <t>exists</t>
-  </si>
-  <si>
-    <t>not exists</t>
-  </si>
-  <si>
-    <t>not in</t>
-  </si>
-  <si>
-    <t>input</t>
-  </si>
-  <si>
-    <t>output</t>
-  </si>
-  <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>correlated exists subquery</t>
-  </si>
-  <si>
-    <t>summary</t>
-  </si>
-  <si>
-    <t>only eq predicates</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>uncorrelated subquery</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>not exists unnested to left join where is null</t>
-  </si>
-  <si>
-    <t>select * from students s where exists (select a.studnr from attend a where a.studnr=26120);</t>
-  </si>
-  <si>
-    <t>select s.* from students s left join (select distinct studnr from attend) a on a.studnr=26120 where a.studnr is not null;</t>
-  </si>
-  <si>
-    <t>select * from students s where not exists (select studnr from attend where studnr=24002);</t>
-  </si>
-  <si>
-    <t>select s.* from students s left join attend a on a.studnr=24002 where a.studnr is null;</t>
-  </si>
-  <si>
-    <t>select s.* from students s left join (select distinct studnr from attend) a on a.studnr=s.studnr where a.studnr is not null;</t>
-  </si>
-  <si>
-    <t>select * from students s where exists (select a.studnr from attend a where a.studnr=s.studnr);</t>
-  </si>
-  <si>
-    <t>exists unnested to left join (select distinct) where is not null; only for eq</t>
-  </si>
-  <si>
-    <t>same as above, only for eq</t>
-  </si>
-  <si>
-    <t>focus on eq subquery connections</t>
-  </si>
-  <si>
-    <t>do we only decorrelate, or also unnest in general</t>
-  </si>
-  <si>
     <t>change in list to simple predicate</t>
+  </si>
+  <si>
+    <t>change where subquery parsing to marker</t>
+  </si>
+  <si>
+    <t>add markers to predicate, add test deparse</t>
+  </si>
+  <si>
+    <t>deparse subqueries at predicate markers</t>
+  </si>
+  <si>
+    <t>use semi join for exists, in-join for in</t>
+  </si>
+  <si>
+    <t>add markers to subquery (in join), don't deparse markers</t>
+  </si>
+  <si>
+    <t>had problem with group by after unnesting</t>
+  </si>
+  <si>
+    <t>"in" in nested boolean</t>
+  </si>
+  <si>
+    <t>Query</t>
+  </si>
+  <si>
+    <t>Can't put m as subquery in from, need to put as cte</t>
+  </si>
+  <si>
+    <t>not exists -&gt; not in</t>
+  </si>
+  <si>
+    <t>subquery with equi predicate -&gt; from subquery with group by</t>
+  </si>
+  <si>
+    <t>exists -&gt; in</t>
+  </si>
+  <si>
+    <t>subquery with complex predicate -&gt; from subquery with group by</t>
+  </si>
+  <si>
+    <t>transformation</t>
+  </si>
+  <si>
+    <t>exists/not exists -&gt; exists with from subquery with group by</t>
   </si>
 </sst>
 </file>
@@ -1062,7 +1012,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1083,18 +1033,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1117,21 +1061,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1150,7 +1085,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1158,12 +1093,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1566,97 +1497,97 @@
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>239</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>245</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>244</v>
-      </c>
       <c r="C14" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>272</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C19" s="4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C20" s="4" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -1667,148 +1598,99 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E917740-AD23-492A-8962-EF2BCDE6AB5A}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" customWidth="1"/>
     <col min="3" max="3" width="29.5703125" customWidth="1"/>
     <col min="4" max="4" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
-        <v>294</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>299</v>
       </c>
       <c r="B1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>306</v>
+      </c>
+      <c r="C8" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>22</v>
+      </c>
+      <c r="B9" s="14" t="s">
         <v>301</v>
       </c>
-      <c r="C1" t="s">
-        <v>298</v>
-      </c>
-      <c r="D1" t="s">
-        <v>299</v>
-      </c>
-      <c r="E1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>295</v>
-      </c>
-      <c r="B2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C2" t="s">
-        <v>313</v>
-      </c>
-      <c r="D2" t="s">
-        <v>314</v>
-      </c>
-      <c r="E2" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>302</v>
-      </c>
-      <c r="C3" t="s">
-        <v>318</v>
-      </c>
-      <c r="D3" t="s">
-        <v>317</v>
-      </c>
-      <c r="E3" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>296</v>
-      </c>
-      <c r="B4" t="s">
-        <v>309</v>
-      </c>
-      <c r="C4" t="s">
-        <v>315</v>
-      </c>
-      <c r="D4" t="s">
-        <v>316</v>
-      </c>
-      <c r="E4" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="15" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G14" t="s">
-        <v>310</v>
-      </c>
-      <c r="H14" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G15" t="s">
-        <v>305</v>
-      </c>
-      <c r="H15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>303</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>321</v>
-      </c>
-      <c r="G16" t="s">
-        <v>306</v>
-      </c>
-      <c r="H16">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>295</v>
-      </c>
-      <c r="B17" t="s">
-        <v>304</v>
-      </c>
-      <c r="G17" t="s">
-        <v>307</v>
-      </c>
-      <c r="H17">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>322</v>
-      </c>
-      <c r="G18" t="s">
-        <v>308</v>
-      </c>
-      <c r="H18">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1818,10 +1700,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C36143C-8755-4841-9383-2CD561E91E02}">
-  <dimension ref="A1:J38"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A26" sqref="A21:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,10 +1736,10 @@
         <v>211</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J1" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1877,10 +1759,10 @@
         <v>192</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1897,7 +1779,7 @@
         <v>208</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1911,7 +1793,7 @@
         <v>203</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1933,13 +1815,13 @@
         <v>196</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>205</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1947,54 +1829,54 @@
         <v>195</v>
       </c>
       <c r="B7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>201</v>
       </c>
       <c r="F7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="B8" t="s">
+        <v>263</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="B8" t="s">
-        <v>264</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>217</v>
-      </c>
       <c r="F8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C10" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" s="9" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F11" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2002,7 +1884,7 @@
         <v>204</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2010,7 +1892,7 @@
         <v>206</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2018,46 +1900,46 @@
         <v>210</v>
       </c>
       <c r="F14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="F15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C16" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="F16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="B20" s="10" t="s">
-        <v>231</v>
-      </c>
       <c r="C20" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -2068,10 +1950,10 @@
         <v>1</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -2082,165 +1964,186 @@
         <v>3</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C23" s="13">
         <v>5</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C24" s="13">
         <v>6</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
-        <v>17</v>
-      </c>
-      <c r="B25" t="s">
-        <v>285</v>
+        <v>21</v>
       </c>
       <c r="C25" s="13">
         <v>7</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C26" s="13">
         <v>8</v>
       </c>
       <c r="I26" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="J26" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="J26" s="9" t="s">
-        <v>248</v>
-      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="13">
-        <v>19</v>
+      <c r="A27" t="s">
+        <v>220</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>251</v>
       </c>
       <c r="C27" s="13">
         <v>9</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="13">
-        <v>20</v>
-      </c>
       <c r="C28" s="13">
         <v>10</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="13">
-        <v>21</v>
-      </c>
-      <c r="C29" s="14">
+      <c r="C29" s="13">
         <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>283</v>
+        <v>297</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="13">
-        <v>22</v>
-      </c>
       <c r="C30" s="13">
+        <v>12</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="13">
         <v>13</v>
       </c>
-      <c r="J30" s="9" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>221</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>252</v>
-      </c>
-      <c r="C31" s="13">
-        <v>14</v>
-      </c>
       <c r="I31" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C32" s="13">
+        <v>14</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="13">
         <v>15</v>
       </c>
-      <c r="I32" s="9" t="s">
-        <v>270</v>
-      </c>
-      <c r="J32" s="9" t="s">
+      <c r="I33" s="9" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="13">
+        <v>16</v>
+      </c>
+      <c r="I34" s="9" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I33" s="9" t="s">
+    <row r="35" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C35" s="13">
+        <v>18</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="13">
+        <v>19</v>
+      </c>
+      <c r="D36" t="s">
+        <v>298</v>
+      </c>
+      <c r="I36" s="12" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="I34" s="9" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="35" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I35" s="9" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="36" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I36" s="12" t="s">
-        <v>276</v>
-      </c>
       <c r="J36" s="9" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="37" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C37" s="6"/>
-      <c r="I37" s="17" t="s">
-        <v>323</v>
+      <c r="I37" s="14" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="38" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C38" s="6"/>
+      <c r="I38" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J39" s="9" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J40" s="9" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="J41" s="9" t="s">
+        <v>294</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2249,6 +2152,18 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E6D5E8-CEF3-46B5-B7DF-339133CE553E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C530AA-EE6D-4730-B7FC-66C1C2338D8E}">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -2651,7 +2566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800A685A-9F16-4D2A-89B8-E0E1402FCD61}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -3019,7 +2934,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D31B28C7-0856-B849-8670-D0B5AB075FAE}">
   <dimension ref="A1:E5"/>
   <sheetViews>

</xml_diff>

<commit_message>
correct tpch21 transformation description
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Uni\DataEngineering\WS22\Guided Research\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA5B1FB-14AF-490E-BC5E-C92108C7276F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C42939C-DCF5-4F9B-9350-C32F9513FA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="804" yWindow="204" windowWidth="17712" windowHeight="12132" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="38670" windowHeight="16470" activeTab="1" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
   <sheets>
     <sheet name="Meeting Notes" sheetId="4" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="315">
   <si>
     <t>paper</t>
   </si>
@@ -944,9 +944,6 @@
     <t>Query</t>
   </si>
   <si>
-    <t>Can't put m as subquery in from, need to put as cte</t>
-  </si>
-  <si>
     <t>not exists -&gt; not in</t>
   </si>
   <si>
@@ -962,9 +959,6 @@
     <t>transformation</t>
   </si>
   <si>
-    <t>exists/not exists -&gt; exists with from subquery with group by</t>
-  </si>
-  <si>
     <t>can also be used by exists/in with complex predicate?</t>
   </si>
   <si>
@@ -1002,6 +996,9 @@
   </si>
   <si>
     <t>needs extra relation in from, only because of "&lt;"/"&gt;"</t>
+  </si>
+  <si>
+    <t>exists/not exists -&gt; cte and left join + null check</t>
   </si>
 </sst>
 </file>
@@ -1039,7 +1036,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1055,6 +1052,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1093,7 +1096,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1112,7 +1115,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1122,6 +1125,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1439,8 +1443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FDCCB2-898C-4E8A-AEF1-A7FCAFD38A4A}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,13 +1600,13 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>304</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>305</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1610,43 +1614,43 @@
         <v>286</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C20" s="4" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>311</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>
@@ -1659,8 +1663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E917740-AD23-492A-8962-EF2BCDE6AB5A}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,7 +1679,7 @@
         <v>295</v>
       </c>
       <c r="B1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C1" t="s">
         <v>41</v>
@@ -1686,7 +1690,7 @@
         <v>227</v>
       </c>
       <c r="B2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1694,10 +1698,10 @@
         <v>228</v>
       </c>
       <c r="B3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C3" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1705,7 +1709,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1713,7 +1717,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1721,7 +1725,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1729,18 +1733,15 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
-        <v>302</v>
-      </c>
-      <c r="C8" t="s">
-        <v>296</v>
+      <c r="B8" s="16" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1748,7 +1749,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1765,7 +1766,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A26" sqref="A21:A26"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
neumann decorrelation  with decoupling
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Uni\DataEngineering\WS22\Guided Research\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680B6F62-4026-49AE-9EEC-3C60E72D37B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01969507-D54D-4157-9087-08DEF224AC0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
+    <workbookView xWindow="3180" yWindow="270" windowWidth="22140" windowHeight="15165" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
   <sheets>
     <sheet name="Meeting Notes" sheetId="4" r:id="rId1"/>
     <sheet name="Tests" sheetId="6" r:id="rId2"/>
-    <sheet name="SQL Parser" sheetId="5" r:id="rId3"/>
-    <sheet name="RA optimizer" sheetId="7" r:id="rId4"/>
-    <sheet name="Papers" sheetId="1" r:id="rId5"/>
-    <sheet name="Parsers" sheetId="2" r:id="rId6"/>
-    <sheet name="Optimizers" sheetId="3" r:id="rId7"/>
+    <sheet name="PSQL Performance" sheetId="8" r:id="rId3"/>
+    <sheet name="SQL Parser" sheetId="5" r:id="rId4"/>
+    <sheet name="RA optimizer" sheetId="7" r:id="rId5"/>
+    <sheet name="Papers" sheetId="1" r:id="rId6"/>
+    <sheet name="Parsers" sheetId="2" r:id="rId7"/>
+    <sheet name="Optimizers" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="374">
   <si>
     <t>paper</t>
   </si>
@@ -1025,9 +1026,6 @@
     <t>What is Tempscan operator in Umbra?</t>
   </si>
   <si>
-    <t>PostreSQL instance with TPCH</t>
-  </si>
-  <si>
     <t>Alex help setup</t>
   </si>
   <si>
@@ -1041,6 +1039,144 @@
   </si>
   <si>
     <t>Instread of tempscan, need to scan table</t>
+  </si>
+  <si>
+    <t>original</t>
+  </si>
+  <si>
+    <t>decorrelated</t>
+  </si>
+  <si>
+    <t>2363,854 ms (00:02,364)</t>
+  </si>
+  <si>
+    <t>2412726,898 ms (40:12,727)</t>
+  </si>
+  <si>
+    <t>Q17</t>
+  </si>
+  <si>
+    <t>TPCH</t>
+  </si>
+  <si>
+    <t>Q22</t>
+  </si>
+  <si>
+    <t>205,010 ms</t>
+  </si>
+  <si>
+    <t>329501,595 ms (05:29,502)</t>
+  </si>
+  <si>
+    <t>Q21</t>
+  </si>
+  <si>
+    <t>498,419 ms</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>Q20</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>https://mariadb.com/kb/en/exists-to-in-optimization/</t>
+  </si>
+  <si>
+    <t>Postgres "not exists" better than "not in" due to null check not in https://explainextended.com/2009/09/16/not-in-vs-not-exists-vs-left-join-is-null-postgresql/</t>
+  </si>
+  <si>
+    <t>dnf</t>
+  </si>
+  <si>
+    <t>1467,400 ms (00:01,467)</t>
+  </si>
+  <si>
+    <t>183,439 ms</t>
+  </si>
+  <si>
+    <t>186,085 ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 226,738 ms</t>
+  </si>
+  <si>
+    <t>147,444 ms</t>
+  </si>
+  <si>
+    <t>PostgreSQL performance discussion</t>
+  </si>
+  <si>
+    <t>PostgreSQL instance with TPCH</t>
+  </si>
+  <si>
+    <t>Neumann algo, how get predicate in first step?</t>
+  </si>
+  <si>
+    <t>error (explicit join before implicit)</t>
+  </si>
+  <si>
+    <t>careful when transforming exists/in</t>
+  </si>
+  <si>
+    <t>08.12.2022</t>
+  </si>
+  <si>
+    <t>First focus on Neumann's algo, then consider exists/in discussion</t>
+  </si>
+  <si>
+    <t>Idea for potential DBIMP project</t>
+  </si>
+  <si>
+    <t>Only missing join predicate and decoupling in Neumann algo</t>
+  </si>
+  <si>
+    <t>Confirm: When decoupling, Neumanns selection is not necessary</t>
+  </si>
+  <si>
+    <t>Q2 needs select distinct, due to non-equi predicates</t>
+  </si>
+  <si>
+    <t>Sideway information passing</t>
+  </si>
+  <si>
+    <t>13.12.2022</t>
+  </si>
+  <si>
+    <t>why umbra doesn't decouple…</t>
+  </si>
+  <si>
+    <t>if "or" an uncorrelated predicate?</t>
+  </si>
+  <si>
+    <t>if +1 an equi correlated predicate?</t>
+  </si>
+  <si>
+    <t>Sideway information passing -&gt; CTE</t>
+  </si>
+  <si>
+    <t>now only supports if attribute names are unique in CTE (with schema, easier to fix this)</t>
+  </si>
+  <si>
+    <t>What to prioritise</t>
+  </si>
+  <si>
+    <t>add schema</t>
+  </si>
+  <si>
+    <t>build UI</t>
+  </si>
+  <si>
+    <t>unnesting 100% (multiple correlations,all subquery operators, ...)</t>
+  </si>
+  <si>
+    <t>clean up c-style pointers</t>
+  </si>
+  <si>
+    <t>visualize RA tree</t>
   </si>
 </sst>
 </file>
@@ -1491,10 +1627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FDCCB2-898C-4E8A-AEF1-A7FCAFD38A4A}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="B24" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1708,18 +1844,18 @@
         <v>319</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>326</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1737,10 +1873,106 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>324</v>
+    </row>
+    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="4" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="4" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="4" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="4" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="4" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="4" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="4" t="s">
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -1751,10 +1983,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E917740-AD23-492A-8962-EF2BCDE6AB5A}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1772,10 +2004,13 @@
         <v>300</v>
       </c>
       <c r="C1" t="s">
+        <v>328</v>
+      </c>
+      <c r="D1" t="s">
+        <v>329</v>
+      </c>
+      <c r="E1" t="s">
         <v>41</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1785,9 +2020,6 @@
       <c r="B2" t="s">
         <v>297</v>
       </c>
-      <c r="E2" t="s">
-        <v>314</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1796,11 +2028,8 @@
       <c r="B3" t="s">
         <v>299</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>301</v>
-      </c>
-      <c r="E3" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1810,6 +2039,12 @@
       <c r="B4" t="s">
         <v>297</v>
       </c>
+      <c r="C4" t="s">
+        <v>348</v>
+      </c>
+      <c r="D4" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
@@ -1818,6 +2053,15 @@
       <c r="B5" s="9" t="s">
         <v>298</v>
       </c>
+      <c r="C5" t="s">
+        <v>346</v>
+      </c>
+      <c r="D5" t="s">
+        <v>347</v>
+      </c>
+      <c r="E5" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
@@ -1826,6 +2070,12 @@
       <c r="B6" t="s">
         <v>297</v>
       </c>
+      <c r="C6" t="s">
+        <v>331</v>
+      </c>
+      <c r="D6" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
@@ -1834,6 +2084,12 @@
       <c r="B7" t="s">
         <v>297</v>
       </c>
+      <c r="C7" t="s">
+        <v>344</v>
+      </c>
+      <c r="D7" t="s">
+        <v>345</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
@@ -1843,6 +2099,12 @@
         <v>316</v>
       </c>
       <c r="C8" t="s">
+        <v>338</v>
+      </c>
+      <c r="D8" t="s">
+        <v>353</v>
+      </c>
+      <c r="E8" t="s">
         <v>317</v>
       </c>
     </row>
@@ -1852,6 +2114,27 @@
       </c>
       <c r="B9" s="9" t="s">
         <v>296</v>
+      </c>
+      <c r="C9" t="s">
+        <v>335</v>
+      </c>
+      <c r="D9" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>315</v>
       </c>
     </row>
   </sheetData>
@@ -1861,6 +2144,105 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D4A399D-CABA-45A5-9450-29512CD5D8FE}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C1" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>228</v>
+      </c>
+      <c r="B2" t="s">
+        <v>348</v>
+      </c>
+      <c r="C2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B3" t="s">
+        <v>346</v>
+      </c>
+      <c r="C3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>332</v>
+      </c>
+      <c r="B4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>340</v>
+      </c>
+      <c r="B5" t="s">
+        <v>344</v>
+      </c>
+      <c r="C5" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>337</v>
+      </c>
+      <c r="B6" t="s">
+        <v>338</v>
+      </c>
+      <c r="C6" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>334</v>
+      </c>
+      <c r="B7" t="s">
+        <v>335</v>
+      </c>
+      <c r="C7" t="s">
+        <v>336</v>
+      </c>
+      <c r="D7" t="s">
+        <v>343</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C36143C-8755-4841-9383-2CD561E91E02}">
   <dimension ref="A1:J41"/>
   <sheetViews>
@@ -2313,7 +2695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E6D5E8-CEF3-46B5-B7DF-339133CE553E}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2325,7 +2707,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54C530AA-EE6D-4730-B7FC-66C1C2338D8E}">
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -2728,7 +3110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800A685A-9F16-4D2A-89B8-E0E1402FCD61}">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -3096,7 +3478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D31B28C7-0856-B849-8670-D0B5AB075FAE}">
   <dimension ref="A1:E5"/>
   <sheetViews>

</xml_diff>

<commit_message>
add extended test cases
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Uni\DataEngineering\WS22\Guided Research\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE6CA366-58AB-4B94-942C-B52336AEAAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0350D40-9D11-4FD6-83E0-07141C5B8814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1044" yWindow="216" windowWidth="17712" windowHeight="12132" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="38670" windowHeight="16470" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
   <sheets>
     <sheet name="Meeting Notes" sheetId="4" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="386">
   <si>
     <t>paper</t>
   </si>
@@ -1186,6 +1186,33 @@
   </si>
   <si>
     <t>add support for TPCH (Q2,17,20)</t>
+  </si>
+  <si>
+    <t>20.12.2022</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>Tests to 100% algorithm</t>
+  </si>
+  <si>
+    <t>outer/semi joins</t>
+  </si>
+  <si>
+    <t>multiple correlations in query</t>
+  </si>
+  <si>
+    <t>Q1/Q2 &amp; TPCH decorrelated (special handling for exists/in)</t>
+  </si>
+  <si>
+    <t>set operations (add to sql parser)</t>
+  </si>
+  <si>
+    <t>Q1 läuft in Umbra nicht (siehe screenshots)</t>
+  </si>
+  <si>
+    <t>mit CTEs geht's schon</t>
   </si>
 </sst>
 </file>
@@ -1636,10 +1663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FDCCB2-898C-4E8A-AEF1-A7FCAFD38A4A}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B32" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1961,27 +1988,27 @@
         <v>368</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C42" s="4" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C43" s="4" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C44" s="4" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C45" s="4" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -1995,6 +2022,45 @@
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C47" s="4" t="s">
         <v>363</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="4" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C51" s="4" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -2008,7 +2074,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
refactored to smart pointers
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Uni\DataEngineering\WS22\Guided Research\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0350D40-9D11-4FD6-83E0-07141C5B8814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C941FE-3993-4EC0-A522-264395623F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-135" yWindow="-135" windowWidth="38670" windowHeight="16470" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="387">
   <si>
     <t>paper</t>
   </si>
@@ -1213,6 +1213,9 @@
   </si>
   <si>
     <t>mit CTEs geht's schon</t>
+  </si>
+  <si>
+    <t>Refactored to smart pointers</t>
   </si>
 </sst>
 </file>
@@ -1663,10 +1666,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FDCCB2-898C-4E8A-AEF1-A7FCAFD38A4A}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2034,32 +2037,37 @@
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="C50" s="4" t="s">
         <v>380</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C50" s="4" t="s">
-        <v>381</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C51" s="4" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C52" s="4" t="s">
         <v>383</v>
-      </c>
-    </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
         <v>378</v>
       </c>
     </row>
@@ -2334,7 +2342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C36143C-8755-4841-9383-2CD561E91E02}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
case 3 for dep join join-pushdown
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyDocs\Uni\DataEngineering\WS22\Guided Research\sql_optimizer\GuidedResearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Guided Research\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C941FE-3993-4EC0-A522-264395623F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612AFD3E-B181-4C78-AFA3-D0BD2536833F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="38670" windowHeight="16470" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="14220" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
   <sheets>
     <sheet name="Meeting Notes" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <sheet name="Optimizers" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="395">
   <si>
     <t>paper</t>
   </si>
@@ -1216,6 +1215,30 @@
   </si>
   <si>
     <t>Refactored to smart pointers</t>
+  </si>
+  <si>
+    <t>10.01.2022</t>
+  </si>
+  <si>
+    <t>toggle whether keep cross products or convert to joins</t>
+  </si>
+  <si>
+    <t>Version mit correlated predicate pushdown -&gt; enables all join pushdown cases</t>
+  </si>
+  <si>
+    <t>18.01.2022</t>
+  </si>
+  <si>
+    <t>Umbra: First unnest, then predicate pushdown</t>
+  </si>
+  <si>
+    <t>In umbra, 3rd join pushdown case doesn't happen…?</t>
+  </si>
+  <si>
+    <t>Join push down all the way (like in umbra), or stop as soon as uncorrelated condition fulfilled?</t>
+  </si>
+  <si>
+    <t>If push dep join all the way down join tree, then subsequent predicate pushdown can potentially push down more correlated predicates into the join tree</t>
   </si>
 </sst>
 </file>
@@ -1666,22 +1689,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FDCCB2-898C-4E8A-AEF1-A7FCAFD38A4A}">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="B47" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="55.5703125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="65.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="24.1796875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="55.54296875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="65.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.81640625" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>176</v>
       </c>
@@ -1692,7 +1715,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>175</v>
       </c>
@@ -1703,7 +1726,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
         <v>179</v>
       </c>
@@ -1711,7 +1734,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
         <v>183</v>
       </c>
@@ -1719,7 +1742,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
         <v>182</v>
       </c>
@@ -1727,7 +1750,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>185</v>
       </c>
@@ -1735,7 +1758,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>189</v>
       </c>
@@ -1743,7 +1766,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>187</v>
       </c>
@@ -1751,7 +1774,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>222</v>
       </c>
@@ -1762,7 +1785,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="4" t="s">
         <v>238</v>
       </c>
@@ -1770,7 +1793,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B11" s="4" t="s">
         <v>244</v>
       </c>
@@ -1778,17 +1801,17 @@
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="11" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>242</v>
       </c>
@@ -1799,7 +1822,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>271</v>
       </c>
@@ -1807,12 +1830,12 @@
         <v>272</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="B16" s="4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>283</v>
       </c>
@@ -1823,7 +1846,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>302</v>
       </c>
@@ -1834,7 +1857,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B19" s="4" t="s">
         <v>286</v>
       </c>
@@ -1842,22 +1865,22 @@
         <v>305</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C20" s="4" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C21" s="4" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B22" s="4" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="B23" s="4" t="s">
         <v>309</v>
       </c>
@@ -1865,12 +1888,12 @@
         <v>311</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B24" s="4" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="B25" s="4" t="s">
         <v>312</v>
       </c>
@@ -1878,7 +1901,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
         <v>319</v>
       </c>
@@ -1889,7 +1912,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B27" s="4" t="s">
         <v>324</v>
       </c>
@@ -1897,7 +1920,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B28" s="4" t="s">
         <v>322</v>
       </c>
@@ -1905,12 +1928,12 @@
         <v>321</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B29" s="4" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B30" s="4" t="s">
         <v>351</v>
       </c>
@@ -1918,7 +1941,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
         <v>355</v>
       </c>
@@ -1929,17 +1952,17 @@
         <v>352</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C32" s="4" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C33" s="4" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="4" t="s">
         <v>350</v>
       </c>
@@ -1947,22 +1970,22 @@
         <v>354</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="4" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B36" s="4" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B37" s="4" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
         <v>362</v>
       </c>
@@ -1973,12 +1996,12 @@
         <v>376</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C39" s="4" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B40" s="4" t="s">
         <v>372</v>
       </c>
@@ -1986,7 +2009,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B41" s="4" t="s">
         <v>368</v>
       </c>
@@ -1994,27 +2017,27 @@
         <v>366</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C42" s="4" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C43" s="4" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C44" s="4" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C45" s="4" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B46" s="4" t="s">
         <v>370</v>
       </c>
@@ -2022,12 +2045,12 @@
         <v>371</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C47" s="4" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
         <v>377</v>
       </c>
@@ -2035,12 +2058,12 @@
         <v>382</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B49" s="4" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B50" s="4" t="s">
         <v>379</v>
       </c>
@@ -2048,17 +2071,17 @@
         <v>380</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C51" s="4" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C52" s="4" t="s">
         <v>383</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B53" s="4" t="s">
         <v>384</v>
       </c>
@@ -2066,9 +2089,41 @@
         <v>385</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B54" s="4" t="s">
         <v>378</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A55" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B56" s="4" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A57" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B58" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -2085,14 +2140,14 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="58.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" customWidth="1"/>
-    <col min="4" max="4" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="58.26953125" customWidth="1"/>
+    <col min="3" max="3" width="29.54296875" customWidth="1"/>
+    <col min="4" max="4" width="27.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>295</v>
       </c>
@@ -2109,7 +2164,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>227</v>
       </c>
@@ -2117,7 +2172,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>228</v>
       </c>
@@ -2128,7 +2183,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -2142,7 +2197,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -2159,7 +2214,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>17</v>
       </c>
@@ -2173,7 +2228,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>20</v>
       </c>
@@ -2187,7 +2242,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>21</v>
       </c>
@@ -2204,7 +2259,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>22</v>
       </c>
@@ -2218,17 +2273,17 @@
         <v>336</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>315</v>
       </c>
@@ -2247,13 +2302,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>333</v>
       </c>
@@ -2264,7 +2319,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>228</v>
       </c>
@@ -2275,7 +2330,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>341</v>
       </c>
@@ -2286,7 +2341,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>332</v>
       </c>
@@ -2297,7 +2352,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>340</v>
       </c>
@@ -2308,7 +2363,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>337</v>
       </c>
@@ -2319,7 +2374,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>334</v>
       </c>
@@ -2346,17 +2401,17 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="2" max="2" width="18.54296875" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
         <v>191</v>
       </c>
@@ -2382,7 +2437,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>192</v>
       </c>
@@ -2405,7 +2460,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>193</v>
       </c>
@@ -2422,7 +2477,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>194</v>
       </c>
@@ -2436,7 +2491,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>202</v>
       </c>
@@ -2450,7 +2505,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>196</v>
       </c>
@@ -2464,7 +2519,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="9" t="s">
         <v>195</v>
       </c>
@@ -2478,7 +2533,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>215</v>
       </c>
@@ -2492,7 +2547,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>264</v>
       </c>
@@ -2503,7 +2558,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C10" s="9" t="s">
         <v>253</v>
       </c>
@@ -2511,7 +2566,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C11" s="9" t="s">
         <v>225</v>
       </c>
@@ -2519,7 +2574,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C12" s="9" t="s">
         <v>204</v>
       </c>
@@ -2527,7 +2582,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C13" s="9" t="s">
         <v>206</v>
       </c>
@@ -2535,7 +2590,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C14" s="9" t="s">
         <v>210</v>
       </c>
@@ -2543,7 +2598,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C15" t="s">
         <v>220</v>
       </c>
@@ -2554,7 +2609,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C16" s="9" t="s">
         <v>281</v>
       </c>
@@ -2562,7 +2617,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>229</v>
       </c>
@@ -2582,7 +2637,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="13">
         <v>2</v>
       </c>
@@ -2596,7 +2651,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="13">
         <v>4</v>
       </c>
@@ -2610,7 +2665,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="13">
         <v>17</v>
       </c>
@@ -2621,7 +2676,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="13">
         <v>20</v>
       </c>
@@ -2632,7 +2687,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="13">
         <v>21</v>
       </c>
@@ -2643,7 +2698,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="13">
         <v>22</v>
       </c>
@@ -2657,7 +2712,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>220</v>
       </c>
@@ -2671,7 +2726,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C28" s="13">
         <v>10</v>
       </c>
@@ -2679,7 +2734,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C29" s="13">
         <v>11</v>
       </c>
@@ -2690,7 +2745,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C30" s="13">
         <v>12</v>
       </c>
@@ -2698,7 +2753,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C31" s="13">
         <v>13</v>
       </c>
@@ -2706,7 +2761,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C32" s="13">
         <v>14</v>
       </c>
@@ -2717,7 +2772,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C33" s="13">
         <v>15</v>
       </c>
@@ -2725,7 +2780,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C34" s="13">
         <v>16</v>
       </c>
@@ -2733,7 +2788,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="35" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C35" s="13">
         <v>18</v>
       </c>
@@ -2741,7 +2796,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="36" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C36" s="13">
         <v>19</v>
       </c>
@@ -2755,13 +2810,13 @@
         <v>282</v>
       </c>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C37" s="6"/>
       <c r="I37" s="9" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.35">
       <c r="C38" s="6"/>
       <c r="I38" s="9" t="s">
         <v>288</v>
@@ -2770,17 +2825,17 @@
         <v>292</v>
       </c>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.35">
       <c r="J39" s="9" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:10" x14ac:dyDescent="0.35">
       <c r="J40" s="9" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:10" x14ac:dyDescent="0.35">
       <c r="J41" s="9" t="s">
         <v>290</v>
       </c>
@@ -2797,7 +2852,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2811,17 +2866,17 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.453125" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" customWidth="1"/>
     <col min="3" max="3" width="38" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="62.85546875" customWidth="1"/>
+    <col min="6" max="6" width="62.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2841,7 +2896,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2858,7 +2913,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2875,7 +2930,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2892,7 +2947,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -2909,7 +2964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -2926,7 +2981,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -2946,7 +3001,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -2966,7 +3021,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -2986,7 +3041,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -3003,7 +3058,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -3020,7 +3075,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -3040,7 +3095,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -3060,7 +3115,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -3077,7 +3132,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -3097,7 +3152,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -3114,7 +3169,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -3134,7 +3189,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -3154,7 +3209,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -3171,7 +3226,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -3214,18 +3269,18 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="49.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>77</v>
       </c>
@@ -3248,7 +3303,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -3268,7 +3323,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -3288,7 +3343,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -3311,7 +3366,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -3334,7 +3389,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -3354,7 +3409,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -3377,7 +3432,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -3400,7 +3455,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>113</v>
       </c>
@@ -3420,7 +3475,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -3440,7 +3495,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>130</v>
       </c>
@@ -3463,7 +3518,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>153</v>
       </c>
@@ -3486,7 +3541,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>157</v>
       </c>
@@ -3509,7 +3564,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>115</v>
       </c>
@@ -3517,7 +3572,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>121</v>
       </c>
@@ -3528,7 +3583,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -3539,7 +3594,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>135</v>
       </c>
@@ -3550,7 +3605,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C26" t="s">
         <v>125</v>
       </c>
@@ -3582,13 +3637,13 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="37.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>136</v>
       </c>
@@ -3605,7 +3660,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -3622,7 +3677,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>142</v>
       </c>
@@ -3636,7 +3691,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>146</v>
       </c>
@@ -3647,7 +3702,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>167</v>
       </c>

</xml_diff>

<commit_message>
decouple multiple dep joins individually
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Guided Research\sql_optimizer\GuidedResearch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{612AFD3E-B181-4C78-AFA3-D0BD2536833F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F99C4EA9-76FF-467D-854D-0FD826612878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="14220" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="402">
   <si>
     <t>paper</t>
   </si>
@@ -1239,6 +1239,27 @@
   </si>
   <si>
     <t>If push dep join all the way down join tree, then subsequent predicate pushdown can potentially push down more correlated predicates into the join tree</t>
+  </si>
+  <si>
+    <t>24.01.2022</t>
+  </si>
+  <si>
+    <t>don't push down correlated predicates (umbra/hyper case)</t>
+  </si>
+  <si>
+    <t>push down correlated predicates, don't decouple</t>
+  </si>
+  <si>
+    <t>push down correlated predicates, decouple</t>
+  </si>
+  <si>
+    <t>benchmark (create tpch query, with different selectivities for left side)</t>
+  </si>
+  <si>
+    <t>decoupling when dep join was split during push down</t>
+  </si>
+  <si>
+    <t>When check if decoupling is possible, only check d attributes in local subquery</t>
   </si>
 </sst>
 </file>
@@ -1681,7 +1702,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1689,10 +1710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FDCCB2-898C-4E8A-AEF1-A7FCAFD38A4A}">
-  <dimension ref="A1:C58"/>
+  <dimension ref="A1:C62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B47" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" topLeftCell="B51" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2124,6 +2145,35 @@
       </c>
       <c r="C58" s="4" t="s">
         <v>394</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A59" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C60" s="4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C61" s="4" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="B62" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>401</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update presentation, text, add results
</commit_message>
<xml_diff>
--- a/GuidedResearch/Project Notes.xlsx
+++ b/GuidedResearch/Project Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Documents\Uni\sql_optimizer\GuidedResearch\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B684B6-C7F8-43B1-B875-B4792FC77DE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{38CE13AA-6B6A-435A-86AB-82C362621070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="14220" activeTab="1" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{066AB142-9725-471A-AC99-EFD3D428F740}"/>
   </bookViews>
   <sheets>
     <sheet name="Meeting Notes" sheetId="4" r:id="rId1"/>
@@ -25,6 +25,7 @@
     <sheet name="Optimizers" sheetId="3" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="506">
   <si>
     <t>paper</t>
   </si>
@@ -1567,6 +1568,63 @@
   </si>
   <si>
     <t>not from like, but from nested query</t>
+  </si>
+  <si>
+    <t>Exists and in -&gt; view with group by</t>
+  </si>
+  <si>
+    <t>keep exists/in</t>
+  </si>
+  <si>
+    <t>ggplot ®</t>
+  </si>
+  <si>
+    <t>welche Visualiserungen Sinn machen</t>
+  </si>
+  <si>
+    <t>improvement to baseline</t>
+  </si>
+  <si>
+    <t>Bericht</t>
+  </si>
+  <si>
+    <t>motivation (warum, wofür, wieso)</t>
+  </si>
+  <si>
+    <t>in sqlite/mariadb/duckDB testen (Alex setzt auf Server auf)</t>
+  </si>
+  <si>
+    <t>Dbs langsam oder spezifisch eingebaut, wollen ein tool für alles (nur sql geht). Show benefits, auch wenn sie implementieren, ist gut für die DB</t>
+  </si>
+  <si>
+    <t>limitations</t>
+  </si>
+  <si>
+    <t>general sql (no card. Estimates, which physical joins, decorrelate back to SQL (declarative))</t>
+  </si>
+  <si>
+    <t>Related work (and DBs)</t>
+  </si>
+  <si>
+    <t>Was/wie gemacht. Implementierungsbericht. Was war schwer (challenges), welche Implementierungsentscheidungen. Was wir können und was nicht (scope)</t>
+  </si>
+  <si>
+    <t>Messungen und Auswertungen</t>
+  </si>
+  <si>
+    <t>Conclusion</t>
+  </si>
+  <si>
+    <t>(School of CIT)</t>
+  </si>
+  <si>
+    <t>Template double column</t>
+  </si>
+  <si>
+    <t>Bericht 1 Woche vor Präsi</t>
+  </si>
+  <si>
+    <t>February</t>
   </si>
 </sst>
 </file>
@@ -1717,7 +1775,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1766,6 +1824,8 @@
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2081,22 +2141,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FDCCB2-898C-4E8A-AEF1-A7FCAFD38A4A}">
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView topLeftCell="A70" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1796875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="55.54296875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="65.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.81640625" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="9.1796875" style="4"/>
+    <col min="1" max="1" width="24.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="55.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="65.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>176</v>
       </c>
@@ -2107,7 +2167,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>175</v>
       </c>
@@ -2118,7 +2178,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>179</v>
       </c>
@@ -2126,7 +2186,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>183</v>
       </c>
@@ -2134,7 +2194,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>182</v>
       </c>
@@ -2142,7 +2202,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>185</v>
       </c>
@@ -2150,7 +2210,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>189</v>
       </c>
@@ -2158,7 +2218,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>187</v>
       </c>
@@ -2166,7 +2226,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>222</v>
       </c>
@@ -2177,7 +2237,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
         <v>238</v>
       </c>
@@ -2185,7 +2245,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>244</v>
       </c>
@@ -2193,17 +2253,17 @@
         <v>245</v>
       </c>
     </row>
-    <row r="12" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="11" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>242</v>
       </c>
@@ -2214,7 +2274,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>271</v>
       </c>
@@ -2222,12 +2282,12 @@
         <v>272</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>283</v>
       </c>
@@ -2238,7 +2298,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>302</v>
       </c>
@@ -2249,7 +2309,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>286</v>
       </c>
@@ -2257,22 +2317,22 @@
         <v>305</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C20" s="4" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>309</v>
       </c>
@@ -2280,12 +2340,12 @@
         <v>311</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>312</v>
       </c>
@@ -2293,7 +2353,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>317</v>
       </c>
@@ -2304,7 +2364,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>322</v>
       </c>
@@ -2312,7 +2372,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>320</v>
       </c>
@@ -2320,12 +2380,12 @@
         <v>319</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>349</v>
       </c>
@@ -2333,7 +2393,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>353</v>
       </c>
@@ -2344,17 +2404,17 @@
         <v>350</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C32" s="4" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C33" s="4" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>348</v>
       </c>
@@ -2362,22 +2422,22 @@
         <v>352</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>360</v>
       </c>
@@ -2388,12 +2448,12 @@
         <v>374</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="C39" s="4" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
         <v>370</v>
       </c>
@@ -2401,7 +2461,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
         <v>366</v>
       </c>
@@ -2409,27 +2469,27 @@
         <v>364</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C42" s="4" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C43" s="4" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C44" s="4" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C45" s="4" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="4" t="s">
         <v>368</v>
       </c>
@@ -2437,12 +2497,12 @@
         <v>369</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C47" s="4" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>375</v>
       </c>
@@ -2450,12 +2510,12 @@
         <v>380</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B50" s="4" t="s">
         <v>377</v>
       </c>
@@ -2463,17 +2523,17 @@
         <v>378</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C51" s="4" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C52" s="4" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B53" s="4" t="s">
         <v>382</v>
       </c>
@@ -2481,12 +2541,12 @@
         <v>383</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B54" s="4" t="s">
         <v>376</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>385</v>
       </c>
@@ -2494,12 +2554,12 @@
         <v>387</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B56" s="4" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>388</v>
       </c>
@@ -2510,7 +2570,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B58" s="4" t="s">
         <v>391</v>
       </c>
@@ -2518,7 +2578,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>393</v>
       </c>
@@ -2529,17 +2589,17 @@
         <v>394</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C60" s="4" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C61" s="4" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B62" s="4" t="s">
         <v>398</v>
       </c>
@@ -2547,7 +2607,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>451</v>
       </c>
@@ -2555,7 +2615,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B64" s="4" t="s">
         <v>453</v>
       </c>
@@ -2563,7 +2623,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="65" spans="2:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B65" s="4" t="s">
         <v>454</v>
       </c>
@@ -2571,7 +2631,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B66" s="4" t="s">
         <v>456</v>
       </c>
@@ -2579,15 +2639,147 @@
         <v>474</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B67" s="4" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" s="4" t="s">
         <v>473</v>
       </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="B69" s="28" t="s">
+        <v>480</v>
+      </c>
+      <c r="C69" s="28"/>
+      <c r="D69" s="28"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B70" s="28" t="s">
+        <v>481</v>
+      </c>
+      <c r="C70" s="28"/>
+      <c r="D70" s="28"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" s="28" t="s">
+        <v>482</v>
+      </c>
+      <c r="C71" s="28"/>
+      <c r="D71" s="28"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B72" s="28" t="s">
+        <v>483</v>
+      </c>
+      <c r="C72" s="28"/>
+      <c r="D72" s="28"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B73" s="28" t="s">
+        <v>484</v>
+      </c>
+      <c r="C73" s="28" t="s">
+        <v>486</v>
+      </c>
+      <c r="D73" s="28"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="29" t="s">
+        <v>487</v>
+      </c>
+      <c r="C74" s="28" t="s">
+        <v>488</v>
+      </c>
+      <c r="D74" s="28"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="28" t="s">
+        <v>489</v>
+      </c>
+      <c r="C75" s="28" t="s">
+        <v>490</v>
+      </c>
+      <c r="D75" s="28"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B76" s="28"/>
+      <c r="C76" s="28" t="s">
+        <v>491</v>
+      </c>
+      <c r="D76" s="28"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B77" s="28" t="s">
+        <v>492</v>
+      </c>
+      <c r="C77" s="28" t="s">
+        <v>493</v>
+      </c>
+      <c r="D77" s="28" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C78" s="28" t="s">
+        <v>494</v>
+      </c>
+      <c r="D78" s="28"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C79" s="28" t="s">
+        <v>496</v>
+      </c>
+      <c r="D79" s="28" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C80" s="28" t="s">
+        <v>498</v>
+      </c>
+      <c r="D80" s="28"/>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C81" s="28" t="s">
+        <v>499</v>
+      </c>
+      <c r="D81" s="28"/>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C82" s="28" t="s">
+        <v>500</v>
+      </c>
+      <c r="D82" s="28"/>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C83" s="28" t="s">
+        <v>501</v>
+      </c>
+      <c r="D83" s="28"/>
+    </row>
+    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C84" s="28" t="s">
+        <v>502</v>
+      </c>
+      <c r="D84" s="28"/>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C85" s="28" t="s">
+        <v>503</v>
+      </c>
+      <c r="D85" s="28"/>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C86" s="28" t="s">
+        <v>504</v>
+      </c>
+      <c r="D86" s="28"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2603,13 +2795,13 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="37.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.81640625" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>136</v>
       </c>
@@ -2626,7 +2818,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>141</v>
       </c>
@@ -2643,7 +2835,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>142</v>
       </c>
@@ -2657,7 +2849,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>146</v>
       </c>
@@ -2668,7 +2860,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>167</v>
       </c>
@@ -2689,26 +2881,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB580FC-3ACC-4C8D-9126-74D667E7CBB0}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7265625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="17.36328125" customWidth="1"/>
-    <col min="3" max="3" width="13.7265625" customWidth="1"/>
-    <col min="4" max="4" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7265625" customWidth="1"/>
-    <col min="6" max="6" width="20.7265625" customWidth="1"/>
-    <col min="7" max="7" width="22.6328125" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="23" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
     <col min="8" max="8" width="43" customWidth="1"/>
-    <col min="10" max="10" width="23.26953125" customWidth="1"/>
+    <col min="10" max="10" width="29.5703125" customWidth="1"/>
+    <col min="11" max="11" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
         <v>331</v>
       </c>
@@ -2740,7 +2933,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="24">
         <v>1</v>
       </c>
@@ -2769,7 +2962,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="24">
         <v>2</v>
       </c>
@@ -2801,7 +2994,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="24">
         <v>3</v>
       </c>
@@ -2830,7 +3023,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="24">
         <v>4</v>
       </c>
@@ -2862,7 +3055,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="24">
         <v>5</v>
       </c>
@@ -2894,7 +3087,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="24">
         <v>6</v>
       </c>
@@ -2919,8 +3112,14 @@
         <f t="shared" si="2"/>
         <v>-0.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J7" s="14" t="s">
+        <v>487</v>
+      </c>
+      <c r="K7" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="24">
         <v>7</v>
       </c>
@@ -2945,8 +3144,14 @@
         <f t="shared" si="2"/>
         <v>-0.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J8" t="s">
+        <v>489</v>
+      </c>
+      <c r="K8" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="24">
         <v>8</v>
       </c>
@@ -2971,8 +3176,11 @@
         <f t="shared" si="2"/>
         <v>-0.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K9" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="24">
         <v>9</v>
       </c>
@@ -2997,8 +3205,17 @@
         <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J10" t="s">
+        <v>492</v>
+      </c>
+      <c r="K10" t="s">
+        <v>493</v>
+      </c>
+      <c r="L10" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="24">
         <v>10</v>
       </c>
@@ -3023,8 +3240,11 @@
         <f t="shared" si="2"/>
         <v>0.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K11" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="24">
         <v>11</v>
       </c>
@@ -3049,8 +3269,14 @@
         <f t="shared" si="2"/>
         <v>-1.7000000000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K12" t="s">
+        <v>496</v>
+      </c>
+      <c r="L12" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="24">
         <v>12</v>
       </c>
@@ -3075,8 +3301,11 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K13" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="24">
         <v>13</v>
       </c>
@@ -3101,8 +3330,11 @@
         <f t="shared" si="2"/>
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K14" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="24">
         <v>14</v>
       </c>
@@ -3127,8 +3359,11 @@
         <f t="shared" si="2"/>
         <v>-0.70000000000000007</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="K15" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="24">
         <v>15</v>
       </c>
@@ -3153,8 +3388,11 @@
         <f t="shared" si="2"/>
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K16" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="24">
         <v>16</v>
       </c>
@@ -3179,8 +3417,11 @@
         <f t="shared" si="2"/>
         <v>1.2</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K17" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="24">
         <v>17</v>
       </c>
@@ -3208,8 +3449,11 @@
       <c r="H18" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K18" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="24">
         <v>18</v>
       </c>
@@ -3234,8 +3478,11 @@
         <f t="shared" si="2"/>
         <v>-0.3</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="K19" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="24">
         <v>19</v>
       </c>
@@ -3261,7 +3508,7 @@
         <v>-0.89999999999999991</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="24">
         <v>20</v>
       </c>
@@ -3290,7 +3537,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="24">
         <v>21</v>
       </c>
@@ -3319,7 +3566,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="24">
         <v>22</v>
       </c>
@@ -3348,7 +3595,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>478</v>
       </c>
@@ -3377,7 +3624,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>477</v>
       </c>
@@ -3403,7 +3650,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="24" t="s">
         <v>476</v>
       </c>
@@ -3429,7 +3676,7 @@
         <v>-32.800000000000004</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="24" t="s">
         <v>470</v>
       </c>
@@ -3455,7 +3702,7 @@
         <v>-403.4</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
         <v>471</v>
       </c>
@@ -3481,7 +3728,7 @@
         <v>-1670.2000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="24" t="s">
         <v>472</v>
       </c>
@@ -3504,10 +3751,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31"/>
     </row>
   </sheetData>
@@ -3550,19 +3797,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E917740-AD23-492A-8962-EF2BCDE6AB5A}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" customWidth="1"/>
-    <col min="2" max="2" width="58.26953125" customWidth="1"/>
-    <col min="3" max="3" width="29.54296875" customWidth="1"/>
-    <col min="4" max="4" width="27.1796875" customWidth="1"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>295</v>
       </c>
@@ -3579,7 +3826,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>227</v>
       </c>
@@ -3587,7 +3834,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>228</v>
       </c>
@@ -3598,7 +3845,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>2</v>
       </c>
@@ -3612,7 +3859,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>4</v>
       </c>
@@ -3629,7 +3876,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>17</v>
       </c>
@@ -3643,7 +3890,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>20</v>
       </c>
@@ -3657,7 +3904,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>21</v>
       </c>
@@ -3674,7 +3921,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>22</v>
       </c>
@@ -3688,7 +3935,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>410</v>
       </c>
@@ -3702,7 +3949,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>402</v>
       </c>
@@ -3713,7 +3960,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>403</v>
       </c>
@@ -3724,7 +3971,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>404</v>
       </c>
@@ -3735,12 +3982,12 @@
         <v>407</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>401</v>
       </c>
@@ -3759,17 +4006,17 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="31.6328125" customWidth="1"/>
-    <col min="4" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="31.5703125" customWidth="1"/>
+    <col min="4" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>431</v>
       </c>
@@ -3804,7 +4051,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" s="20" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>326</v>
       </c>
@@ -3815,7 +4062,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="20" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" s="20" customFormat="1" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>400</v>
       </c>
@@ -3853,7 +4100,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="20" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" s="20" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>402</v>
       </c>
@@ -3891,7 +4138,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="20" customFormat="1" ht="29.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" s="20" customFormat="1" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>403</v>
       </c>
@@ -3902,7 +4149,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="6" spans="1:12" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" s="20" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>404</v>
       </c>
@@ -3919,7 +4166,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>447</v>
       </c>
@@ -3927,22 +4174,22 @@
         <v>450</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>449</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>445</v>
       </c>
@@ -3961,13 +4208,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>331</v>
       </c>
@@ -3978,7 +4225,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>228</v>
       </c>
@@ -3989,7 +4236,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>339</v>
       </c>
@@ -4000,7 +4247,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>330</v>
       </c>
@@ -4011,7 +4258,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>338</v>
       </c>
@@ -4022,7 +4269,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>335</v>
       </c>
@@ -4033,7 +4280,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>332</v>
       </c>
@@ -4060,17 +4307,17 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
-    <col min="2" max="2" width="18.54296875" customWidth="1"/>
-    <col min="3" max="3" width="18.1796875" customWidth="1"/>
-    <col min="4" max="5" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>191</v>
       </c>
@@ -4096,7 +4343,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>192</v>
       </c>
@@ -4119,7 +4366,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>193</v>
       </c>
@@ -4136,7 +4383,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>194</v>
       </c>
@@ -4150,7 +4397,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>202</v>
       </c>
@@ -4164,7 +4411,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>196</v>
       </c>
@@ -4178,7 +4425,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>195</v>
       </c>
@@ -4192,7 +4439,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>215</v>
       </c>
@@ -4206,7 +4453,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>264</v>
       </c>
@@ -4217,7 +4464,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C10" s="9" t="s">
         <v>253</v>
       </c>
@@ -4225,7 +4472,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C11" s="9" t="s">
         <v>225</v>
       </c>
@@ -4233,7 +4480,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C12" s="9" t="s">
         <v>204</v>
       </c>
@@ -4241,7 +4488,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C13" s="9" t="s">
         <v>206</v>
       </c>
@@ -4249,7 +4496,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C14" s="9" t="s">
         <v>210</v>
       </c>
@@ -4257,7 +4504,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>220</v>
       </c>
@@ -4268,7 +4515,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C16" s="9" t="s">
         <v>281</v>
       </c>
@@ -4276,7 +4523,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>229</v>
       </c>
@@ -4296,7 +4543,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="13">
         <v>2</v>
       </c>
@@ -4310,7 +4557,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="13">
         <v>4</v>
       </c>
@@ -4324,7 +4571,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="13">
         <v>17</v>
       </c>
@@ -4335,7 +4582,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="13">
         <v>20</v>
       </c>
@@ -4346,7 +4593,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="13">
         <v>21</v>
       </c>
@@ -4357,7 +4604,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="13">
         <v>22</v>
       </c>
@@ -4371,7 +4618,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>220</v>
       </c>
@@ -4385,7 +4632,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C28" s="13">
         <v>10</v>
       </c>
@@ -4393,7 +4640,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C29" s="13">
         <v>11</v>
       </c>
@@ -4404,7 +4651,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C30" s="13">
         <v>12</v>
       </c>
@@ -4412,7 +4659,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C31" s="13">
         <v>13</v>
       </c>
@@ -4420,7 +4667,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C32" s="13">
         <v>14</v>
       </c>
@@ -4431,7 +4678,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C33" s="13">
         <v>15</v>
       </c>
@@ -4439,7 +4686,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C34" s="13">
         <v>16</v>
       </c>
@@ -4447,7 +4694,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="35" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="13">
         <v>18</v>
       </c>
@@ -4455,7 +4702,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="36" spans="3:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="13">
         <v>19</v>
       </c>
@@ -4469,13 +4716,13 @@
         <v>282</v>
       </c>
     </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C37" s="6"/>
       <c r="I37" s="9" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C38" s="6"/>
       <c r="I38" s="9" t="s">
         <v>288</v>
@@ -4484,17 +4731,17 @@
         <v>292</v>
       </c>
     </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
       <c r="J39" s="9" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
       <c r="J40" s="9" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
       <c r="J41" s="9" t="s">
         <v>290</v>
       </c>
@@ -4509,9 +4756,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E6D5E8-CEF3-46B5-B7DF-339133CE553E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="H1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4525,17 +4772,17 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.453125" customWidth="1"/>
-    <col min="2" max="2" width="17.1796875" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="38" customWidth="1"/>
-    <col min="4" max="4" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="62.81640625" customWidth="1"/>
+    <col min="6" max="6" width="62.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -4555,7 +4802,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -4572,7 +4819,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -4589,7 +4836,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -4606,7 +4853,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -4623,7 +4870,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -4640,7 +4887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -4660,7 +4907,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -4680,7 +4927,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -4700,7 +4947,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -4717,7 +4964,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -4734,7 +4981,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -4754,7 +5001,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -4774,7 +5021,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -4791,7 +5038,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -4811,7 +5058,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -4828,7 +5075,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -4848,7 +5095,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>66</v>
       </c>
@@ -4868,7 +5115,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -4885,7 +5132,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>73</v>
       </c>
@@ -4928,18 +5175,18 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="49.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="7" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>77</v>
       </c>
@@ -4962,7 +5209,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -4982,7 +5229,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -5002,7 +5249,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -5025,7 +5272,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -5048,7 +5295,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -5068,7 +5315,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -5091,7 +5338,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>106</v>
       </c>
@@ -5114,7 +5361,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>113</v>
       </c>
@@ -5134,7 +5381,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>123</v>
       </c>
@@ -5154,7 +5401,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>130</v>
       </c>
@@ -5177,7 +5424,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>153</v>
       </c>
@@ -5200,7 +5447,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>157</v>
       </c>
@@ -5223,7 +5470,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>115</v>
       </c>
@@ -5231,7 +5478,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>121</v>
       </c>
@@ -5242,7 +5489,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>117</v>
       </c>
@@ -5253,7 +5500,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>135</v>
       </c>
@@ -5264,7 +5511,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>125</v>
       </c>

</xml_diff>